<commit_message>
Reduced layer count from 6 to 4
As originally suggested by @smunaut for reDIP SID.
</commit_message>
<xml_diff>
--- a/documentation/reDIP-SX-BOM.xlsx
+++ b/documentation/reDIP-SX-BOM.xlsx
@@ -7,22 +7,22 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="reDIP-SX-kicost. " sheetId="1" r:id="rId1"/>
+    <sheet name="reDIP-SX-BOM. " sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="arrow_part_data">'reDIP-SX-kicost. '!$K$5:$O$37</definedName>
-    <definedName name="BoardQty">'reDIP-SX-kicost. '!$J$1</definedName>
-    <definedName name="digikey_part_data">'reDIP-SX-kicost. '!$P$5:$T$37</definedName>
-    <definedName name="farnell_part_data">'reDIP-SX-kicost. '!$U$5:$Y$37</definedName>
-    <definedName name="global_part_data">'reDIP-SX-kicost. '!$A$5:$J$37</definedName>
-    <definedName name="lcsc_part_data">'reDIP-SX-kicost. '!$Z$5:$AD$37</definedName>
-    <definedName name="mouser_part_data">'reDIP-SX-kicost. '!$AE$5:$AI$37</definedName>
-    <definedName name="newark_part_data">'reDIP-SX-kicost. '!$AJ$5:$AN$37</definedName>
-    <definedName name="PURCHASE_DESCRIPTION">'reDIP-SX-kicost. '!$J$40</definedName>
-    <definedName name="rs_part_data">'reDIP-SX-kicost. '!$AO$5:$AS$37</definedName>
-    <definedName name="tme_part_data">'reDIP-SX-kicost. '!$AT$5:$AX$37</definedName>
-    <definedName name="TotalCost">'reDIP-SX-kicost. '!$J$3</definedName>
-    <definedName name="USD_GBP">'reDIP-SX-kicost. '!$C$40</definedName>
+    <definedName name="arrow_part_data">'reDIP-SX-BOM. '!$K$5:$O$37</definedName>
+    <definedName name="BoardQty">'reDIP-SX-BOM. '!$J$1</definedName>
+    <definedName name="digikey_part_data">'reDIP-SX-BOM. '!$P$5:$T$37</definedName>
+    <definedName name="farnell_part_data">'reDIP-SX-BOM. '!$U$5:$Y$37</definedName>
+    <definedName name="global_part_data">'reDIP-SX-BOM. '!$A$5:$J$37</definedName>
+    <definedName name="lcsc_part_data">'reDIP-SX-BOM. '!$Z$5:$AD$37</definedName>
+    <definedName name="mouser_part_data">'reDIP-SX-BOM. '!$AE$5:$AI$37</definedName>
+    <definedName name="newark_part_data">'reDIP-SX-BOM. '!$AJ$5:$AN$37</definedName>
+    <definedName name="PURCHASE_DESCRIPTION">'reDIP-SX-BOM. '!$J$40</definedName>
+    <definedName name="rs_part_data">'reDIP-SX-BOM. '!$AO$5:$AS$37</definedName>
+    <definedName name="tme_part_data">'reDIP-SX-BOM. '!$AT$5:$AX$37</definedName>
+    <definedName name="TotalCost">'reDIP-SX-BOM. '!$J$3</definedName>
+    <definedName name="USD_GBP">'reDIP-SX-BOM. '!$C$40</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -862,19 +862,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="P7" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not normally stocked.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="R7" authorId="0">
       <text>
         <r>
@@ -910,16 +897,16 @@
   Qty  -  Unit£  -  Ext£
 ================
      1   £1.10      £1.10
-    10   £1.10     £11.00
+    10   £1.04     £10.40
     50   £1.01     £50.50
-   100   £0.87     £87.20
+   100   £0.83     £83.20
    250   £0.76    £191.25
    500   £0.59    £294.00
   1000   £0.68    £676.00
   1800   £0.62  £1,108.80
   2500   £0.57  £1,430.00
   4500   £0.57  £2,565.00
-  9000   £0.60  £5,436.00
+  9000   £0.57  £5,112.00
  45000   £0.57 £25,470.00</t>
         </r>
       </text>
@@ -949,12 +936,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $1.69      $1.69
-    10   $1.53     $15.30
-    50   $1.53     $76.50
-   100   $1.23    $123.00
-  1000   $0.83    $832.00
- 10000   $0.72  $7,170.00</t>
+     1   $1.61      $1.61
+    10   $1.37     $13.70
+    50   $1.37     $68.50
+   100   $1.10    $110.00
+  1000   $0.89    $888.00
+ 10000   $0.80  $8,000.00</t>
         </r>
       </text>
     </comment>
@@ -991,6 +978,7 @@
   Qty  -  Unit£  -  Ext£
 ================
      1   £1.28      £1.28
+     5 £956.09  £4,780.45
     25   £1.09     £27.25
     50   £0.96     £48.00
    100   £0.83     £83.00
@@ -1099,12 +1087,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-    10   $0.06      $0.64
-   100   $0.05      $4.94
-   300   $0.05     $14.04
-  1000   $0.04     $44.20
-  5000   $0.04    $215.50
- 10000   $0.04    $425.00</t>
+    10   $0.06      $0.58
+   100   $0.05      $4.56
+   300   $0.04     $12.99
+  1000   $0.04     $41.10
+  5000   $0.04    $200.50
+ 10000   $0.04    $396.00</t>
         </r>
       </text>
     </comment>
@@ -1198,6 +1186,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="U9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not normally stocked.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="W9" authorId="0">
       <text>
         <r>
@@ -1242,6 +1243,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="AJ9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not normally stocked.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="AL9" authorId="0">
       <text>
         <r>
@@ -1258,7 +1272,7 @@
     25   $0.11      $2.82
     50   $0.10      $5.25
    100   $0.10      $9.70
- 15000   $0.05    $810.00</t>
+ 15000   $0.05    $795.00</t>
         </r>
       </text>
     </comment>
@@ -1321,12 +1335,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     5   $0.12      $0.59
-    50   $0.09      $4.30
-   150   $0.08     $12.02
-   500   $0.07     $37.10
-  2500   $0.07    $179.00
-  5000   $0.07    $351.50</t>
+     5   $0.12      $0.60
+    50   $0.09      $4.40
+   150   $0.08     $12.32
+   500   $0.08     $38.05
+  2500   $0.07    $183.50
+  5000   $0.07    $360.50</t>
         </r>
       </text>
     </comment>
@@ -1430,12 +1444,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-    10   $0.06      $0.61
-   100   $0.05      $4.53
-   300   $0.04     $12.72
-  1000   $0.04     $39.50
-  5000   $0.04    $191.00
- 10000   $0.04    $376.00</t>
+    10   $0.06      $0.63
+   100   $0.05      $4.69
+   300   $0.04     $13.20
+  1000   $0.04     $41.10
+  5000   $0.04    $199.00
+ 10000   $0.04    $392.00</t>
         </r>
       </text>
     </comment>
@@ -1675,9 +1689,9 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.39      $0.39
-    10   $0.26      $2.55
-    50   $0.26     $12.75
-   100   $0.14     $13.80
+    10   $0.28      $2.76
+    50   $0.28     $13.80
+   100   $0.16     $15.70
   1000   $0.08     $84.00
  10000   $0.06    $580.00</t>
         </r>
@@ -1750,12 +1764,12 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.64      £3.21
-    10   £0.52      £5.19
-   100   £0.33     £32.60
-   150   £0.33     £48.90
-   500   £0.24    £120.00
-  3000   £0.20    £609.00</t>
+     5   £0.65      £3.27
+    10   £0.55      £5.48
+   100   £0.34     £33.60
+   150   £0.34     £50.40
+   500   £0.24    £121.50
+  3000   £0.20    £612.00</t>
         </r>
       </text>
     </comment>
@@ -1814,8 +1828,8 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.70      $0.70
-    10   $0.62      $6.19
-   100   $0.42     $42.10
+    10   $0.61      $6.10
+   100   $0.42     $42.30
    500   $0.35    $176.50
   3000   $0.21    $639.00
   9000   $0.19  $1,710.00
@@ -1856,12 +1870,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.71      $0.71
-    10   $0.46      $4.65
-   100   $0.31     $30.77
-  1000   $0.24    $237.55
-  2000   $0.21    $429.30
-  6000   $0.20  $1,215.00</t>
+     1   $0.72      $0.72
+    10   $0.48      $4.75
+   100   $0.31     $31.45
+  1000   $0.24    $242.82
+  2000   $0.22    $438.84
+  6000   $0.21  $1,242.00</t>
         </r>
       </text>
     </comment>
@@ -1909,12 +1923,12 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.66      $0.66
-    10   $0.43      $4.30
-    50   $0.43     $21.50
-   100   $0.28     $28.20
-  1000   $0.22    $222.00
- 10000   $0.18  $1,820.00</t>
+     1   $0.68      $0.68
+    10   $0.44      $4.41
+    50   $0.44     $22.05
+   100   $0.29     $28.90
+  1000   $0.23    $228.00
+ 10000   $0.19  $1,860.00</t>
         </r>
       </text>
     </comment>
@@ -1964,19 +1978,6 @@
     25   £0.20      £5.09
    100   £0.17     £17.32
    500   £0.16     £78.95</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P16" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not normally stocked.</t>
         </r>
       </text>
     </comment>
@@ -2529,19 +2530,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="P23" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This part is listed but is not normally stocked.</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="R23" authorId="0">
       <text>
         <r>
@@ -2606,11 +2594,11 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.10      $0.10
-    10   $0.02      $0.25
-    50   $0.02      $1.25
-   100   $0.01      $0.80
-  1000   $0.00      $5.00
- 10000   $0.00     $30.00</t>
+    10   $0.03      $0.31
+    50   $0.03      $1.55
+   100   $0.01      $1.40
+  1000   $0.01      $7.00
+ 10000   $0.00     $50.00</t>
         </r>
       </text>
     </comment>
@@ -2745,10 +2733,10 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.10      $0.10
-    10   $0.03      $0.27
-    50   $0.03      $1.35
-   100   $0.01      $1.10
-  1000   $0.00      $5.00
+    10   $0.03      $0.28
+    50   $0.03      $1.40
+   100   $0.01      $1.20
+  1000   $0.01      $6.00
  10000   $0.00     $30.00</t>
         </r>
       </text>
@@ -2779,22 +2767,6 @@
   Qty  -  Unit$  -  Ext$
 ================
  45000   $0.00    $180.00</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="AQ24" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Qty/Price Breaks (GBP):
-  Qty  -  Unit£  -  Ext£
-================
- 15000   £0.01     £90.00</t>
         </r>
       </text>
     </comment>
@@ -2968,10 +2940,10 @@
   Qty  -  Unit$  -  Ext$
 ================
      1   $0.10      $0.10
-    10   $0.03      $0.27
-    50   $0.03      $1.35
-   100   $0.01      $1.10
-  1000   $0.00      $5.00
+    10   $0.03      $0.28
+    50   $0.03      $1.40
+   100   $0.01      $1.20
+  1000   $0.01      $6.00
  10000   $0.00     $30.00</t>
         </r>
       </text>
@@ -3017,18 +2989,16 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.35      $0.35
-    10   $0.26      $2.58
-    25   $0.23      $5.64
-   100   $0.15     $14.60
-   250   $0.12     $30.21
-   500   $0.10     $48.34
-  1000   $0.07     $74.12
-  3000   $0.06    $193.35
-  6000   $0.06    $348.00
- 15000   $0.05    $773.40
- 30000   $0.05  $1,450.20
- 75000   $0.05  $3,420.00</t>
+     1   $0.46      $0.46
+    10   $0.34      $3.43
+    25   $0.30      $7.51
+   100   $0.19     $19.45
+   250   $0.16     $40.25
+   500   $0.13     $64.40
+  1000   $0.10     $98.74
+  3000   $0.09    $257.58
+  6000   $0.08    $463.62
+ 15000   $0.07  $1,063.05</t>
         </r>
       </text>
     </comment>
@@ -3085,19 +3055,13 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     5   $0.31      $1.56
-    10   $0.24      $2.40
-    25   $0.16      $4.10
-    50   $0.14      $6.80
-   100   $0.11     $11.40
-   250   $0.09     $22.75
-   500   $0.08     $38.00
-  1000   $0.06     $63.00
-  3000   $0.05    $150.00
- 12000   $0.05    $600.00
- 18000   $0.04    $756.00
- 48000   $0.04  $1,824.00
- 90000   $0.04  $3,240.00</t>
+     5   $0.36      $1.82
+    10   $0.30      $2.96
+   100   $0.14     $13.80
+  6000   $0.06    $354.00
+  9000   $0.06    $495.00
+ 24000   $0.05  $1,224.00
+ 45000   $0.05  $2,160.00</t>
         </r>
       </text>
     </comment>
@@ -3335,6 +3299,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="P30" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This part is listed but is not normally stocked.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="R30" authorId="0">
       <text>
         <r>
@@ -3347,17 +3324,14 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $0.54      $0.54
-    10   $0.44      $4.38
-    25   $0.40     $10.03
-   100   $0.30     $29.85
-   250   $0.27     $67.63
-   500   $0.22    $111.94
-  1000   $0.17    $167.90
-  3000   $0.15    $461.73
-  6000   $0.14    $867.48
- 15000   $0.14  $2,028.90
- 30000   $0.13  $3,960.00</t>
+     1   $0.47      $0.47
+    10   $0.40      $4.02
+    25   $0.38      $9.39
+   100   $0.30     $30.04
+   250   $0.28     $69.73
+   500   $0.24    $118.00
+  1000   $0.18    $182.36
+  3000   $0.18    $531.30</t>
         </r>
       </text>
     </comment>
@@ -3373,15 +3347,12 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     5   £0.42      £2.11
-    10   £0.31      £3.09
-   100   £0.14     £14.20
-   150   £0.14     £21.30
-   500   £0.10     £52.50
-  3000   £0.09    £274.20
-  9000   £0.09    £793.80
- 24000   £0.09  £2,042.40
- 45000   £0.08  £3,762.00</t>
+     5   £0.59      £2.94
+    10   £0.43      £4.28
+   100   £0.21     £21.40
+   150   £0.21     £32.10
+   500   £0.15     £73.00
+  3000   £0.13    £399.00</t>
         </r>
       </text>
     </comment>
@@ -3418,21 +3389,16 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     5   $0.58      $2.91
-    10   $0.45      $4.47
-    25   $0.37      $9.30
-    50   $0.31     $15.65
-   100   $0.26     $26.20
-   250   $0.22     $55.75
-   500   $0.18     $91.00
-  1000   $0.16    $155.00
-  3000   $0.14    $423.00
-  6000   $0.13    $792.00
- 12000   $0.12  $1,452.00
- 18000   $0.12  $2,178.00
- 24000   $0.12  $2,880.00
- 30000   $0.12  $3,600.00
-300000   $0.12 $36,000.00</t>
+     5   $0.61      $3.06
+    10   $0.46      $4.55
+   100   $0.23     $23.30
+  3000   $0.14    $414.00
+  6000   $0.14    $816.00
+ 12000   $0.13  $1,608.00
+ 18000   $0.13  $2,376.00
+ 24000   $0.13  $3,120.00
+ 30000   $0.13  $3,870.00
+300000   $0.13 $38,100.00</t>
         </r>
       </text>
     </comment>
@@ -3556,8 +3522,8 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $3.54      $3.54
-    10   $3.50     $35.00</t>
+     1   $3.63      $3.63
+  5000   $3.50 $17,498.25</t>
         </r>
       </text>
     </comment>
@@ -3586,14 +3552,11 @@
           <t>Qty/Price Breaks (GBP):
   Qty  -  Unit£  -  Ext£
 ================
-     1   £2.90      £2.90
-    10   £2.17     £21.70
-    25   £2.05     £51.25
-    50   £1.92     £96.00
-   100   £1.80    £180.00
-   250   £1.61    £402.50
-   500   £1.54    £770.00
-  1000   £1.28  £1,280.00</t>
+     1   £3.61      £3.61
+    10   £2.74     £27.40
+    25   £2.69     £67.25
+    50   £2.64    £132.00
+   100   £2.59    £259.00</t>
         </r>
       </text>
     </comment>
@@ -3626,7 +3589,7 @@
     10   $3.22     $32.20
     50   $3.04    $152.00
    100   $2.64    $264.00
-  1000   $2.55  $2,550.00
+  1000   $2.59  $2,590.00
  10000   $2.54 $25,400.00</t>
         </r>
       </text>
@@ -3656,13 +3619,8 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $3.83      $3.83
-    10   $3.13     $31.30
-    25   $2.94     $73.50
-    50   $2.76    $138.00
-   100   $2.58    $258.00
-   250   $2.31    $577.50
-  2450   $2.31  $5,659.50</t>
+     1   $3.45      $3.45
+  5000   $3.33 $16,650.00</t>
         </r>
       </text>
     </comment>
@@ -3870,11 +3828,11 @@
           <t>Qty/Price Breaks (USD):
   Qty  -  Unit$  -  Ext$
 ================
-     1   $2.13      $2.13
-    10   $1.98     $19.80
-    25   $1.85     $46.25
-    50   $1.73     $86.50
-   100   $1.61    $161.00</t>
+     1   $2.16      $2.16
+    10   $2.01     $20.10
+    25   $1.89     $47.25
+    50   $1.76     $88.00
+   100   $1.64    $164.00</t>
         </r>
       </text>
     </comment>
@@ -4176,7 +4134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="321">
   <si>
     <t>Global Part Info</t>
   </si>
@@ -4259,8 +4217,8 @@
     <t>GRM033C80J105ME05D</t>
   </si>
   <si>
-    <t>C11-C14,C18-C22: 1.55V DC AUDIO
-C2,C24,C28: 1.2V DC</t>
+    <t>C2,C24,C28: 1.2V DC
+C11-C14,C18-C22: 1.55V DC AUDIO</t>
   </si>
   <si>
     <t>C4</t>
@@ -4594,7 +4552,10 @@
     <t>NXP</t>
   </si>
   <si>
-    <t>ALTERNATIVE PART #: SGTL5000XNLA3R2</t>
+    <t>SGTL5000XNLA3R2</t>
+  </si>
+  <si>
+    <t>ALTERNATIVE PART #: SGTL5000XNLA3</t>
   </si>
   <si>
     <t>U5</t>
@@ -4702,7 +4663,7 @@
     <t>Prj date:</t>
   </si>
   <si>
-    <t>lø. 01. mai 2021 kl. 22.55 +0200</t>
+    <t>to. 13. mai 2021 kl. 20.42 +0200</t>
   </si>
   <si>
     <t>Board Qty:</t>
@@ -4717,7 +4678,7 @@
     <t>$ date:</t>
   </si>
   <si>
-    <t>2021-05-01 22:55:19</t>
+    <t>2021-05-13 20:42:43</t>
   </si>
   <si>
     <t>Arrow</t>
@@ -4741,12 +4702,12 @@
     <t>WM4893CT-ND</t>
   </si>
   <si>
+    <t>490-14595-1-ND</t>
+  </si>
+  <si>
     <t>NonStk</t>
   </si>
   <si>
-    <t>490-14595-1-ND</t>
-  </si>
-  <si>
     <t>490-13218-1-ND</t>
   </si>
   <si>
@@ -4816,7 +4777,7 @@
     <t>FSA221UMXTR-ND</t>
   </si>
   <si>
-    <t>SGTL5000XNLA3-ND</t>
+    <t>568-13255-1-ND</t>
   </si>
   <si>
     <t>1965-ESP32-PICO-V3-02-ND</t>
@@ -4894,7 +4855,7 @@
     <t>3614346</t>
   </si>
   <si>
-    <t>2308050</t>
+    <t>2776032</t>
   </si>
   <si>
     <t>3387002</t>
@@ -5005,7 +4966,7 @@
     <t>512FSA221UMX</t>
   </si>
   <si>
-    <t>841SGTL5000XNLA3</t>
+    <t>841SGTL5000XNLA3R2</t>
   </si>
   <si>
     <t>356ESP32PICOV302</t>
@@ -5080,7 +5041,7 @@
     <t>84AC7230</t>
   </si>
   <si>
-    <t>14R9111</t>
+    <t>31AC6932</t>
   </si>
   <si>
     <t>66AH5403</t>
@@ -5092,7 +5053,7 @@
     <t>RS Components</t>
   </si>
   <si>
-    <t>7595325</t>
+    <t>2182169</t>
   </si>
   <si>
     <t>1851581</t>
@@ -5108,9 +5069,6 @@
   </si>
   <si>
     <t>1797111</t>
-  </si>
-  <si>
-    <t>1797103</t>
   </si>
   <si>
     <t>1797101</t>
@@ -5217,18 +5175,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF909090"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -5310,7 +5268,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -5371,10 +5329,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -5780,13 +5738,13 @@
   <sheetData>
     <row r="1" spans="1:50">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="J1" s="3">
         <v>100</v>
@@ -5794,13 +5752,13 @@
     </row>
     <row r="2" spans="1:50">
       <c r="A2" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="J2" s="4">
         <f>TotalCost/BoardQty</f>
@@ -5809,13 +5767,13 @@
     </row>
     <row r="3" spans="1:50">
       <c r="A3" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="J3" s="5">
         <f>SUM(J7:J37)</f>
@@ -5888,10 +5846,10 @@
     </row>
     <row r="4" spans="1:50">
       <c r="A4" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:50">
@@ -5908,49 +5866,49 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="8" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="L5" s="8"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
       <c r="P5" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
       <c r="S5" s="9"/>
       <c r="T5" s="9"/>
       <c r="U5" s="10" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="V5" s="10"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
       <c r="AC5" s="11"/>
       <c r="AD5" s="11"/>
       <c r="AE5" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF5" s="12"/>
       <c r="AG5" s="12"/>
       <c r="AH5" s="12"/>
       <c r="AI5" s="12"/>
       <c r="AJ5" s="13" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AK5" s="13"/>
       <c r="AL5" s="13"/>
       <c r="AM5" s="13"/>
       <c r="AN5" s="13"/>
       <c r="AO5" s="14" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AP5" s="14"/>
       <c r="AQ5" s="14"/>
@@ -5996,10 +5954,10 @@
         <v>9</v>
       </c>
       <c r="K6" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="M6" s="16" t="s">
         <v>8</v>
@@ -6008,13 +5966,13 @@
         <v>9</v>
       </c>
       <c r="O6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="P6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="R6" s="16" t="s">
         <v>8</v>
@@ -6023,13 +5981,13 @@
         <v>9</v>
       </c>
       <c r="T6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="U6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="V6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="U6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="V6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="W6" s="16" t="s">
         <v>8</v>
@@ -6038,13 +5996,13 @@
         <v>9</v>
       </c>
       <c r="Y6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="Z6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AA6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="Z6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="AA6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="AB6" s="16" t="s">
         <v>8</v>
@@ -6053,13 +6011,13 @@
         <v>9</v>
       </c>
       <c r="AD6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="AE6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AF6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="AE6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>8</v>
@@ -6068,13 +6026,13 @@
         <v>9</v>
       </c>
       <c r="AI6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="AJ6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="AJ6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="AK6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="AL6" s="16" t="s">
         <v>8</v>
@@ -6083,13 +6041,13 @@
         <v>9</v>
       </c>
       <c r="AN6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="AO6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AP6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="AO6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="AP6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="AQ6" s="16" t="s">
         <v>8</v>
@@ -6098,13 +6056,13 @@
         <v>9</v>
       </c>
       <c r="AS6" s="16" t="s">
+        <v>184</v>
+      </c>
+      <c r="AT6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="AU6" s="16" t="s">
         <v>183</v>
-      </c>
-      <c r="AT6" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="AU6" s="16" t="s">
-        <v>182</v>
       </c>
       <c r="AV6" s="16" t="s">
         <v>8</v>
@@ -6113,7 +6071,7 @@
         <v>9</v>
       </c>
       <c r="AX6" s="16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:50">
@@ -6147,8 +6105,8 @@
         <f>iferror(H7*I7,"")</f>
         <v>0</v>
       </c>
-      <c r="P7" s="19" t="s">
-        <v>187</v>
+      <c r="P7" s="17">
+        <v>24423</v>
       </c>
       <c r="R7" s="18">
         <f>iferror(lookup(if(Q7="",H7,Q7),{0,1,10,25,100,250,500,1800},{0.0,1.61,1.448,1.3656,1.1636,1.0926,0.95602,0.8604}),"")</f>
@@ -6158,39 +6116,39 @@
         <f>iferror(if(Q7="",H7,Q7)*R7,"")</f>
         <v>0</v>
       </c>
-      <c r="T7" s="20" t="s">
-        <v>186</v>
+      <c r="T7" s="19" t="s">
+        <v>187</v>
       </c>
       <c r="U7" s="17">
-        <v>14432</v>
+        <v>11357</v>
       </c>
       <c r="W7" s="18">
-        <f>iferror(USD_GBP*lookup(if(V7="",H7,V7),{0,1,10,50,100,250,500,1000,1800,2500,4500,9000,45000},{0.0,1.1,1.1,1.01,0.872,0.765,0.588,0.676,0.616,0.572,0.57,0.604,0.566}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V7="",H7,V7),{0,1,10,50,100,250,500,1000,1800,2500,4500,9000,45000},{0.0,1.1,1.04,1.01,0.832,0.765,0.588,0.676,0.616,0.572,0.57,0.568,0.566}),"")</f>
         <v>0</v>
       </c>
       <c r="X7" s="18">
         <f>iferror(if(V7="",H7,V7)*W7,"")</f>
         <v>0</v>
       </c>
-      <c r="Y7" s="20" t="s">
-        <v>218</v>
-      </c>
-      <c r="AE7" s="19" t="s">
-        <v>187</v>
+      <c r="Y7" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="AE7" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG7" s="18">
-        <f>iferror(lookup(if(AF7="",H7,AF7),{0,1,10,50,100,1000,10000},{0.0,1.69,1.53,1.53,1.23,0.832,0.717}),"")</f>
+        <f>iferror(lookup(if(AF7="",H7,AF7),{0,1,10,50,100,1000,10000},{0.0,1.61,1.37,1.37,1.1,0.888,0.8}),"")</f>
         <v>0</v>
       </c>
       <c r="AH7" s="18">
         <f>iferror(if(AF7="",H7,AF7)*AG7,"")</f>
         <v>0</v>
       </c>
-      <c r="AI7" s="20" t="s">
-        <v>253</v>
+      <c r="AI7" s="19" t="s">
+        <v>254</v>
       </c>
       <c r="AJ7" s="17">
-        <v>13470</v>
+        <v>10232</v>
       </c>
       <c r="AL7" s="18">
         <f>iferror(lookup(if(AK7="",H7,AK7),{0,1,10,25,50,100,250},{0.0,1.4,1.4,1.31,1.21,1.12,1.05}),"")</f>
@@ -6200,25 +6158,25 @@
         <f>iferror(if(AK7="",H7,AK7)*AL7,"")</f>
         <v>0</v>
       </c>
-      <c r="AN7" s="20" t="s">
-        <v>281</v>
+      <c r="AN7" s="19" t="s">
+        <v>282</v>
       </c>
       <c r="AO7" s="17">
         <v>8762</v>
       </c>
       <c r="AQ7" s="18">
-        <f>iferror(USD_GBP*lookup(if(AP7="",H7,AP7),{0,1,25,50,100,250},{0.0,1.28,1.09,0.96,0.83,0.77}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(AP7="",H7,AP7),{0,1,5,25,50,100,250},{0.0,1.28,956.09,1.09,0.96,0.83,0.77}),"")</f>
         <v>0</v>
       </c>
       <c r="AR7" s="18">
         <f>iferror(if(AP7="",H7,AP7)*AQ7,"")</f>
         <v>0</v>
       </c>
-      <c r="AS7" s="20" t="s">
-        <v>304</v>
-      </c>
-      <c r="AT7" s="19" t="s">
-        <v>187</v>
+      <c r="AS7" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="AT7" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AV7" s="18">
         <f>iferror(USD_GBP*lookup(if(AU7="",H7,AU7),{0,1,1800},{0.0,0.59777,0.59777}),"")</f>
@@ -6228,7 +6186,7 @@
         <f>iferror(if(AU7="",H7,AU7)*AV7,"")</f>
         <v>0</v>
       </c>
-      <c r="AX7" s="20" t="s">
+      <c r="AX7" s="19" t="s">
         <v>316</v>
       </c>
     </row>
@@ -6266,8 +6224,8 @@
         <f>iferror(H8*I8,"")</f>
         <v>0</v>
       </c>
-      <c r="P8" s="19" t="s">
-        <v>187</v>
+      <c r="P8" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R8" s="18">
         <f>iferror(lookup(if(Q8="",H8,Q8),{0,1,10,50,100,500,1000,2500,5000,10000},{0.0,0.29,0.198,0.119,0.1005,0.06876,0.06084,0.05819,0.0529,0.05026}),"")</f>
@@ -6277,11 +6235,11 @@
         <f>iferror(if(Q8="",H8,Q8)*R8,"")</f>
         <v>0</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="19" t="s">
         <v>188</v>
       </c>
       <c r="U8" s="17">
-        <v>9990</v>
+        <v>9420</v>
       </c>
       <c r="W8" s="18">
         <f>iferror(USD_GBP*lookup(if(V8="",H8,V8),{0,1,10,100,150,500,2500,5000,10000,50000},{0.0,0.128,0.128,0.0638,0.0638,0.0495,0.0319,0.0292,0.0264,0.022}),"")</f>
@@ -6291,25 +6249,25 @@
         <f>iferror(if(V8="",H8,V8)*W8,"")</f>
         <v>0</v>
       </c>
-      <c r="Y8" s="20" t="s">
-        <v>219</v>
+      <c r="Y8" s="19" t="s">
+        <v>220</v>
       </c>
       <c r="Z8" s="17">
-        <v>3280</v>
+        <v>10720</v>
       </c>
       <c r="AB8" s="18">
-        <f>iferror(lookup(if(AA8="",H8,AA8),{0,1,10,100,300,1000,5000,10000},{0.0,0.0635,0.0635,0.0494,0.0468,0.0442,0.0431,0.0425}),"")</f>
+        <f>iferror(lookup(if(AA8="",H8,AA8),{0,1,10,100,300,1000,5000,10000},{0.0,0.0579,0.0579,0.0456,0.0433,0.0411,0.0401,0.0396}),"")</f>
         <v>0</v>
       </c>
       <c r="AC8" s="18">
         <f>iferror(if(AA8="",H8,AA8)*AB8,"")</f>
         <v>0</v>
       </c>
-      <c r="AD8" s="20" t="s">
-        <v>242</v>
-      </c>
-      <c r="AE8" s="19" t="s">
-        <v>187</v>
+      <c r="AD8" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="AE8" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG8" s="18">
         <f>iferror(lookup(if(AF8="",H8,AF8),{0,1,10,50,100,1000,10000},{0.0,0.26,0.174,0.174,0.099,0.061,0.043}),"")</f>
@@ -6319,11 +6277,11 @@
         <f>iferror(if(AF8="",H8,AF8)*AG8,"")</f>
         <v>0</v>
       </c>
-      <c r="AI8" s="20" t="s">
-        <v>254</v>
+      <c r="AI8" s="19" t="s">
+        <v>255</v>
       </c>
       <c r="AJ8" s="17">
-        <v>9990</v>
+        <v>9420</v>
       </c>
       <c r="AL8" s="18">
         <f>iferror(lookup(if(AK8="",H8,AK8),{0,1,10,25,50,100},{0.0,0.174,0.174,0.149,0.124,0.099}),"")</f>
@@ -6333,8 +6291,8 @@
         <f>iferror(if(AK8="",H8,AK8)*AL8,"")</f>
         <v>0</v>
       </c>
-      <c r="AN8" s="20" t="s">
-        <v>282</v>
+      <c r="AN8" s="19" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:50">
@@ -6371,8 +6329,8 @@
         <f>iferror(H9*I9,"")</f>
         <v>0</v>
       </c>
-      <c r="P9" s="19" t="s">
-        <v>187</v>
+      <c r="P9" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R9" s="18">
         <f>iferror(lookup(if(Q9="",H9,Q9),{0,1,10,50,100,500,1000,2500,5000,15000},{0.0,0.25,0.172,0.115,0.0978,0.069,0.06038,0.0575,0.05319,0.04773}),"")</f>
@@ -6382,11 +6340,11 @@
         <f>iferror(if(Q9="",H9,Q9)*R9,"")</f>
         <v>0</v>
       </c>
-      <c r="T9" s="20" t="s">
+      <c r="T9" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="U9" s="20" t="s">
         <v>189</v>
-      </c>
-      <c r="U9" s="17">
-        <v>30000</v>
       </c>
       <c r="W9" s="18">
         <f>iferror(USD_GBP*lookup(if(V9="",H9,V9),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.218,0.218,0.137,0.137,0.103,0.0727,0.0606,0.0594,0.051}),"")</f>
@@ -6396,11 +6354,11 @@
         <f>iferror(if(V9="",H9,V9)*W9,"")</f>
         <v>0</v>
       </c>
-      <c r="Y9" s="20" t="s">
-        <v>220</v>
+      <c r="Y9" s="19" t="s">
+        <v>221</v>
       </c>
       <c r="Z9" s="17">
-        <v>3440</v>
+        <v>2820</v>
       </c>
       <c r="AB9" s="18">
         <f>iferror(lookup(if(AA9="",H9,AA9),{0,1,20,200,600,2000,10000,20000},{0.0,0.0208,0.0208,0.0161,0.0153,0.0144,0.0141,0.0139}),"")</f>
@@ -6410,22 +6368,22 @@
         <f>iferror(if(AA9="",H9,AA9)*AB9,"")</f>
         <v>0</v>
       </c>
-      <c r="AD9" s="20" t="s">
-        <v>243</v>
-      </c>
-      <c r="AJ9" s="17">
-        <v>30000</v>
+      <c r="AD9" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="AJ9" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL9" s="18">
-        <f>iferror(lookup(if(AK9="",H9,AK9),{0,1,10,25,50,100,15000},{0.0,0.121,0.121,0.113,0.105,0.097,0.054}),"")</f>
+        <f>iferror(lookup(if(AK9="",H9,AK9),{0,1,10,25,50,100,15000},{0.0,0.121,0.121,0.113,0.105,0.097,0.053}),"")</f>
         <v>0</v>
       </c>
       <c r="AM9" s="18">
         <f>iferror(if(AK9="",H9,AK9)*AL9,"")</f>
         <v>0</v>
       </c>
-      <c r="AN9" s="20" t="s">
-        <v>283</v>
+      <c r="AN9" s="19" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:50">
@@ -6463,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="P10" s="17">
-        <v>903983</v>
+        <v>167093</v>
       </c>
       <c r="R10" s="18">
         <f>iferror(lookup(if(Q10="",H10,Q10),{0,1,10,50,100,500,1000,2500,5000,10000},{0.0,0.44,0.307,0.215,0.1842,0.13818,0.11668,0.11054,0.1044,0.09826}),"")</f>
@@ -6473,11 +6431,11 @@
         <f>iferror(if(Q10="",H10,Q10)*R10,"")</f>
         <v>0</v>
       </c>
-      <c r="T10" s="20" t="s">
-        <v>190</v>
+      <c r="T10" s="19" t="s">
+        <v>191</v>
       </c>
       <c r="U10" s="17">
-        <v>50000</v>
+        <v>12334</v>
       </c>
       <c r="W10" s="18">
         <f>iferror(USD_GBP*lookup(if(V10="",H10,V10),{0,1,10,100,150,500,2500,5000,10000,50000},{0.0,0.187,0.187,0.151,0.151,0.0842,0.0797,0.074,0.0718,0.0615}),"")</f>
@@ -6487,25 +6445,25 @@
         <f>iferror(if(V10="",H10,V10)*W10,"")</f>
         <v>0</v>
       </c>
-      <c r="Y10" s="20" t="s">
-        <v>221</v>
+      <c r="Y10" s="19" t="s">
+        <v>222</v>
       </c>
       <c r="Z10" s="17">
-        <v>180195</v>
+        <v>309950</v>
       </c>
       <c r="AB10" s="18">
-        <f>iferror(lookup(if(AA10="",H10,AA10),{0,1,5,50,150,500,2500,5000},{0.0,0.1179,0.1179,0.0859,0.0801,0.0742,0.0716,0.0703}),"")</f>
+        <f>iferror(lookup(if(AA10="",H10,AA10),{0,1,5,50,150,500,2500,5000},{0.0,0.1209,0.1209,0.0881,0.0821,0.0761,0.0734,0.0721}),"")</f>
         <v>0</v>
       </c>
       <c r="AC10" s="18">
         <f>iferror(if(AA10="",H10,AA10)*AB10,"")</f>
         <v>0</v>
       </c>
-      <c r="AD10" s="20" t="s">
-        <v>244</v>
+      <c r="AD10" s="19" t="s">
+        <v>245</v>
       </c>
       <c r="AE10" s="17">
-        <v>155342</v>
+        <v>2944</v>
       </c>
       <c r="AG10" s="18">
         <f>iferror(lookup(if(AF10="",H10,AF10),{0,1,10,50,100,1000,10000},{0.0,0.42,0.206,0.206,0.177,0.112,0.094}),"")</f>
@@ -6515,11 +6473,11 @@
         <f>iferror(if(AF10="",H10,AF10)*AG10,"")</f>
         <v>0</v>
       </c>
-      <c r="AI10" s="20" t="s">
-        <v>255</v>
+      <c r="AI10" s="19" t="s">
+        <v>256</v>
       </c>
       <c r="AJ10" s="17">
-        <v>50000</v>
+        <v>12584</v>
       </c>
       <c r="AL10" s="18">
         <f>iferror(lookup(if(AK10="",H10,AK10),{0,1,10,25,50,100,10000},{0.0,0.227,0.227,0.216,0.205,0.194,0.11}),"")</f>
@@ -6529,8 +6487,8 @@
         <f>iferror(if(AK10="",H10,AK10)*AL10,"")</f>
         <v>0</v>
       </c>
-      <c r="AN10" s="20" t="s">
-        <v>284</v>
+      <c r="AN10" s="19" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="11" spans="1:50">
@@ -6568,7 +6526,7 @@
         <v>0</v>
       </c>
       <c r="P11" s="17">
-        <v>3743048</v>
+        <v>2244493</v>
       </c>
       <c r="R11" s="18">
         <f>iferror(lookup(if(Q11="",H11,Q11),{0,1,10,50,100,500,1000,2500,5000,10000},{0.0,0.19,0.129,0.0776,0.0656,0.04484,0.03968,0.03795,0.0345,0.03278}),"")</f>
@@ -6578,8 +6536,8 @@
         <f>iferror(if(Q11="",H11,Q11)*R11,"")</f>
         <v>0</v>
       </c>
-      <c r="T11" s="20" t="s">
-        <v>191</v>
+      <c r="T11" s="19" t="s">
+        <v>192</v>
       </c>
       <c r="U11" s="17">
         <v>140000</v>
@@ -6592,25 +6550,25 @@
         <f>iferror(if(V11="",H11,V11)*W11,"")</f>
         <v>0</v>
       </c>
-      <c r="Y11" s="20" t="s">
-        <v>222</v>
+      <c r="Y11" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="Z11" s="17">
-        <v>2990</v>
+        <v>1990</v>
       </c>
       <c r="AB11" s="18">
-        <f>iferror(lookup(if(AA11="",H11,AA11),{0,1,10,100,300,1000,5000,10000},{0.0,0.0611,0.0611,0.0453,0.0424,0.0395,0.0382,0.0376}),"")</f>
+        <f>iferror(lookup(if(AA11="",H11,AA11),{0,1,10,100,300,1000,5000,10000},{0.0,0.0627,0.0627,0.0469,0.044,0.0411,0.0398,0.0392}),"")</f>
         <v>0</v>
       </c>
       <c r="AC11" s="18">
         <f>iferror(if(AA11="",H11,AA11)*AB11,"")</f>
         <v>0</v>
       </c>
-      <c r="AD11" s="20" t="s">
-        <v>245</v>
+      <c r="AD11" s="19" t="s">
+        <v>246</v>
       </c>
       <c r="AE11" s="17">
-        <v>1634310</v>
+        <v>1392179</v>
       </c>
       <c r="AG11" s="18">
         <f>iferror(lookup(if(AF11="",H11,AF11),{0,1,10,50,100,1000,10000},{0.0,0.18,0.075,0.075,0.063,0.038,0.031}),"")</f>
@@ -6620,11 +6578,11 @@
         <f>iferror(if(AF11="",H11,AF11)*AG11,"")</f>
         <v>0</v>
       </c>
-      <c r="AI11" s="20" t="s">
-        <v>256</v>
+      <c r="AI11" s="19" t="s">
+        <v>257</v>
       </c>
       <c r="AJ11" s="17">
-        <v>150000</v>
+        <v>160000</v>
       </c>
       <c r="AL11" s="18">
         <f>iferror(lookup(if(AK11="",H11,AK11),{0,1,10,25,50,100,10000,20000},{0.0,0.173,0.173,0.144,0.116,0.087,0.033,0.032}),"")</f>
@@ -6634,8 +6592,8 @@
         <f>iferror(if(AK11="",H11,AK11)*AL11,"")</f>
         <v>0</v>
       </c>
-      <c r="AN11" s="20" t="s">
-        <v>285</v>
+      <c r="AN11" s="19" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:50">
@@ -6673,7 +6631,7 @@
         <v>0</v>
       </c>
       <c r="P12" s="17">
-        <v>2181765</v>
+        <v>3852454</v>
       </c>
       <c r="R12" s="18">
         <f>iferror(lookup(if(Q12="",H12,Q12),{0,1,10,50,100,500,1000,2500,5000,15000},{0.0,0.1,0.034,0.0186,0.0152,0.01086,0.00854,0.00776,0.00714,0.00621}),"")</f>
@@ -6683,8 +6641,8 @@
         <f>iferror(if(Q12="",H12,Q12)*R12,"")</f>
         <v>0</v>
       </c>
-      <c r="T12" s="20" t="s">
-        <v>192</v>
+      <c r="T12" s="19" t="s">
+        <v>193</v>
       </c>
       <c r="U12" s="17">
         <v>120000</v>
@@ -6697,11 +6655,11 @@
         <f>iferror(if(V12="",H12,V12)*W12,"")</f>
         <v>0</v>
       </c>
-      <c r="Y12" s="20" t="s">
-        <v>223</v>
+      <c r="Y12" s="19" t="s">
+        <v>224</v>
       </c>
       <c r="Z12" s="17">
-        <v>20800</v>
+        <v>20200</v>
       </c>
       <c r="AB12" s="18">
         <f>iferror(lookup(if(AA12="",H12,AA12),{0,1,50,500,1500,5000,25000,50000},{0.0,0.0035,0.0035,0.0026,0.0024,0.0022,0.0022,0.0021}),"")</f>
@@ -6711,11 +6669,11 @@
         <f>iferror(if(AA12="",H12,AA12)*AB12,"")</f>
         <v>0</v>
       </c>
-      <c r="AD12" s="20" t="s">
-        <v>246</v>
+      <c r="AD12" s="19" t="s">
+        <v>247</v>
       </c>
       <c r="AE12" s="17">
-        <v>301000</v>
+        <v>570198</v>
       </c>
       <c r="AG12" s="18">
         <f>iferror(lookup(if(AF12="",H12,AF12),{0,1,10,50,100,1000,10000},{0.0,0.1,0.018,0.018,0.015,0.009,0.007}),"")</f>
@@ -6725,8 +6683,8 @@
         <f>iferror(if(AF12="",H12,AF12)*AG12,"")</f>
         <v>0</v>
       </c>
-      <c r="AI12" s="20" t="s">
-        <v>257</v>
+      <c r="AI12" s="19" t="s">
+        <v>258</v>
       </c>
       <c r="AJ12" s="17">
         <v>120000</v>
@@ -6739,8 +6697,8 @@
         <f>iferror(if(AK12="",H12,AK12)*AL12,"")</f>
         <v>0</v>
       </c>
-      <c r="AN12" s="20" t="s">
-        <v>286</v>
+      <c r="AN12" s="19" t="s">
+        <v>287</v>
       </c>
       <c r="AO12" s="17">
         <v>7000</v>
@@ -6753,8 +6711,8 @@
         <f>iferror(if(AP12="",H12,AP12)*AQ12,"")</f>
         <v>0</v>
       </c>
-      <c r="AS12" s="20" t="s">
-        <v>305</v>
+      <c r="AS12" s="19" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="13" spans="1:50">
@@ -6789,7 +6747,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="17">
-        <v>32181</v>
+        <v>23799</v>
       </c>
       <c r="R13" s="18">
         <f>iferror(lookup(if(Q13="",H13,Q13),{0,1,10,100,500,1000,2000,5000,10000,30000,50000,100000},{0.0,0.34,0.251,0.142,0.09404,0.0721,0.0627,0.05643,0.05016,0.04703,0.0417,0.04125}),"")</f>
@@ -6799,11 +6757,11 @@
         <f>iferror(if(Q13="",H13,Q13)*R13,"")</f>
         <v>0</v>
       </c>
-      <c r="T13" s="20" t="s">
-        <v>193</v>
-      </c>
-      <c r="U13" s="19" t="s">
-        <v>187</v>
+      <c r="T13" s="19" t="s">
+        <v>194</v>
+      </c>
+      <c r="U13" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W13" s="18">
         <f>iferror(USD_GBP*lookup(if(V13="",H13,V13),{0,1,10000},{0.0,0.042,0.042}),"")</f>
@@ -6813,25 +6771,25 @@
         <f>iferror(if(V13="",H13,V13)*W13,"")</f>
         <v>0</v>
       </c>
-      <c r="Y13" s="20" t="s">
-        <v>224</v>
+      <c r="Y13" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AE13" s="17">
-        <v>249</v>
+        <v>118</v>
       </c>
       <c r="AG13" s="18">
-        <f>iferror(lookup(if(AF13="",H13,AF13),{0,1,10,50,100,1000,10000},{0.0,0.39,0.255,0.255,0.138,0.084,0.058}),"")</f>
+        <f>iferror(lookup(if(AF13="",H13,AF13),{0,1,10,50,100,1000,10000},{0.0,0.39,0.276,0.276,0.157,0.084,0.058}),"")</f>
         <v>0</v>
       </c>
       <c r="AH13" s="18">
         <f>iferror(if(AF13="",H13,AF13)*AG13,"")</f>
         <v>0</v>
       </c>
-      <c r="AI13" s="20" t="s">
-        <v>258</v>
-      </c>
-      <c r="AJ13" s="19" t="s">
-        <v>187</v>
+      <c r="AI13" s="19" t="s">
+        <v>259</v>
+      </c>
+      <c r="AJ13" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL13" s="18">
         <f>iferror(lookup(if(AK13="",H13,AK13),{0,1,5,10,100,500,1000,2500},{0.0,0.36,0.36,0.276,0.154,0.136,0.118,0.103}),"")</f>
@@ -6841,8 +6799,8 @@
         <f>iferror(if(AK13="",H13,AK13)*AL13,"")</f>
         <v>0</v>
       </c>
-      <c r="AN13" s="20" t="s">
-        <v>287</v>
+      <c r="AN13" s="19" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="14" spans="1:50">
@@ -6877,7 +6835,7 @@
         <v>0</v>
       </c>
       <c r="P14" s="17">
-        <v>23415</v>
+        <v>23210</v>
       </c>
       <c r="R14" s="18">
         <f>iferror(lookup(if(Q14="",H14,Q14),{0,1,10,100,500,1000,3000},{0.0,0.6,0.525,0.4023,0.318,0.2625,0.2625}),"")</f>
@@ -6887,22 +6845,22 @@
         <f>iferror(if(Q14="",H14,Q14)*R14,"")</f>
         <v>0</v>
       </c>
-      <c r="T14" s="20" t="s">
-        <v>194</v>
+      <c r="T14" s="19" t="s">
+        <v>195</v>
       </c>
       <c r="U14" s="17">
-        <v>10184</v>
+        <v>8800</v>
       </c>
       <c r="W14" s="18">
-        <f>iferror(USD_GBP*lookup(if(V14="",H14,V14),{0,1,5,10,100,150,500,3000},{0.0,0.642,0.642,0.519,0.326,0.326,0.24,0.203}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V14="",H14,V14),{0,1,5,10,100,150,500,3000},{0.0,0.654,0.654,0.548,0.336,0.336,0.243,0.204}),"")</f>
         <v>0</v>
       </c>
       <c r="X14" s="18">
         <f>iferror(if(V14="",H14,V14)*W14,"")</f>
         <v>0</v>
       </c>
-      <c r="Y14" s="20" t="s">
-        <v>225</v>
+      <c r="Y14" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="Z14" s="17">
         <v>3073</v>
@@ -6915,11 +6873,11 @@
         <f>iferror(if(AA14="",H14,AA14)*AB14,"")</f>
         <v>0</v>
       </c>
-      <c r="AD14" s="20" t="s">
-        <v>247</v>
+      <c r="AD14" s="19" t="s">
+        <v>248</v>
       </c>
       <c r="AE14" s="17">
-        <v>631</v>
+        <v>714</v>
       </c>
       <c r="AG14" s="18">
         <f>iferror(lookup(if(AF14="",H14,AF14),{0,1,10,50,100,1000,10000},{0.0,0.6,0.517,0.517,0.358,0.255,0.21}),"")</f>
@@ -6929,22 +6887,22 @@
         <f>iferror(if(AF14="",H14,AF14)*AG14,"")</f>
         <v>0</v>
       </c>
-      <c r="AI14" s="20" t="s">
-        <v>259</v>
+      <c r="AI14" s="19" t="s">
+        <v>260</v>
       </c>
       <c r="AJ14" s="17">
-        <v>442</v>
+        <v>392</v>
       </c>
       <c r="AL14" s="18">
-        <f>iferror(lookup(if(AK14="",H14,AK14),{0,1,10,100,500,3000,9000,24000,45000},{0.0,0.7,0.619,0.421,0.353,0.213,0.19,0.184,0.172}),"")</f>
+        <f>iferror(lookup(if(AK14="",H14,AK14),{0,1,10,100,500,3000,9000,24000,45000},{0.0,0.7,0.61,0.423,0.353,0.213,0.19,0.184,0.172}),"")</f>
         <v>0</v>
       </c>
       <c r="AM14" s="18">
         <f>iferror(if(AK14="",H14,AK14)*AL14,"")</f>
         <v>0</v>
       </c>
-      <c r="AN14" s="20" t="s">
-        <v>288</v>
+      <c r="AN14" s="19" t="s">
+        <v>289</v>
       </c>
       <c r="AO14" s="17">
         <v>2450</v>
@@ -6957,8 +6915,8 @@
         <f>iferror(if(AP14="",H14,AP14)*AQ14,"")</f>
         <v>0</v>
       </c>
-      <c r="AS14" s="20" t="s">
-        <v>306</v>
+      <c r="AS14" s="19" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="15" spans="1:50">
@@ -6996,21 +6954,21 @@
         <v>0</v>
       </c>
       <c r="P15" s="17">
-        <v>24663</v>
+        <v>24063</v>
       </c>
       <c r="R15" s="18">
-        <f>iferror(lookup(if(Q15="",H15,Q15),{0,1,10,100,1000,2000,6000},{0.0,0.71,0.465,0.3077,0.23755,0.21465,0.2025}),"")</f>
+        <f>iferror(lookup(if(Q15="",H15,Q15),{0,1,10,100,1000,2000,6000},{0.0,0.72,0.475,0.3145,0.24282,0.21942,0.207}),"")</f>
         <v>0</v>
       </c>
       <c r="S15" s="18">
         <f>iferror(if(Q15="",H15,Q15)*R15,"")</f>
         <v>0</v>
       </c>
-      <c r="T15" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="U15" s="19" t="s">
-        <v>187</v>
+      <c r="T15" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="U15" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W15" s="18">
         <f>iferror(USD_GBP*lookup(if(V15="",H15,V15),{0,1,10,100,500},{0.0,0.683,0.451,0.347,0.299}),"")</f>
@@ -7020,25 +6978,25 @@
         <f>iferror(if(V15="",H15,V15)*W15,"")</f>
         <v>0</v>
       </c>
-      <c r="Y15" s="20" t="s">
-        <v>226</v>
+      <c r="Y15" s="19" t="s">
+        <v>227</v>
       </c>
       <c r="AE15" s="17">
         <v>28018</v>
       </c>
       <c r="AG15" s="18">
-        <f>iferror(lookup(if(AF15="",H15,AF15),{0,1,10,50,100,1000,10000},{0.0,0.66,0.43,0.43,0.282,0.222,0.182}),"")</f>
+        <f>iferror(lookup(if(AF15="",H15,AF15),{0,1,10,50,100,1000,10000},{0.0,0.68,0.441,0.441,0.289,0.228,0.186}),"")</f>
         <v>0</v>
       </c>
       <c r="AH15" s="18">
         <f>iferror(if(AF15="",H15,AF15)*AG15,"")</f>
         <v>0</v>
       </c>
-      <c r="AI15" s="20" t="s">
-        <v>260</v>
-      </c>
-      <c r="AJ15" s="19" t="s">
-        <v>187</v>
+      <c r="AI15" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="AJ15" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL15" s="18">
         <f>iferror(lookup(if(AK15="",H15,AK15),{0,1,10000},{0.0,0.222,0.222}),"")</f>
@@ -7048,8 +7006,8 @@
         <f>iferror(if(AK15="",H15,AK15)*AL15,"")</f>
         <v>0</v>
       </c>
-      <c r="AN15" s="20" t="s">
-        <v>289</v>
+      <c r="AN15" s="19" t="s">
+        <v>290</v>
       </c>
       <c r="AT15" s="17">
         <v>1979</v>
@@ -7062,7 +7020,7 @@
         <f>iferror(if(AU15="",H15,AU15)*AV15,"")</f>
         <v>0</v>
       </c>
-      <c r="AX15" s="20" t="s">
+      <c r="AX15" s="19" t="s">
         <v>317</v>
       </c>
     </row>
@@ -7100,8 +7058,8 @@
         <f>iferror(H16*I16,"")</f>
         <v>0</v>
       </c>
-      <c r="P16" s="19" t="s">
-        <v>187</v>
+      <c r="P16" s="17">
+        <v>7155</v>
       </c>
       <c r="R16" s="18">
         <f>iferror(lookup(if(Q16="",H16,Q16),{0,1,10,25,50,100,250,500,1500,3000,7500,10500},{0.0,1.53,1.386,1.3008,1.2444,1.1878,1.07464,0.9898,0.82012,0.79184,0.75225,0.73528}),"")</f>
@@ -7111,11 +7069,11 @@
         <f>iferror(if(Q16="",H16,Q16)*R16,"")</f>
         <v>0</v>
       </c>
-      <c r="T16" s="20" t="s">
-        <v>196</v>
-      </c>
-      <c r="AE16" s="19" t="s">
-        <v>187</v>
+      <c r="T16" s="19" t="s">
+        <v>197</v>
+      </c>
+      <c r="AE16" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG16" s="18">
         <f>iferror(lookup(if(AF16="",H16,AF16),{0,1,10,50,100,1000,10000},{0.0,1.51,1.23,1.23,1.17,0.839,0.728}),"")</f>
@@ -7125,11 +7083,11 @@
         <f>iferror(if(AF16="",H16,AF16)*AG16,"")</f>
         <v>0</v>
       </c>
-      <c r="AI16" s="20" t="s">
-        <v>261</v>
+      <c r="AI16" s="19" t="s">
+        <v>262</v>
       </c>
       <c r="AO16" s="17">
-        <v>78</v>
+        <v>46</v>
       </c>
       <c r="AQ16" s="18">
         <f>iferror(USD_GBP*lookup(if(AP16="",H16,AP16),{0,1,4,20,100,200},{0.0,5.57,5.31,5.04,4.78,4.55}),"")</f>
@@ -7139,8 +7097,8 @@
         <f>iferror(if(AP16="",H16,AP16)*AQ16,"")</f>
         <v>0</v>
       </c>
-      <c r="AS16" s="20" t="s">
-        <v>307</v>
+      <c r="AS16" s="19" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="17" spans="1:50">
@@ -7185,8 +7143,8 @@
         <f>iferror(if(Q17="",H17,Q17)*R17,"")</f>
         <v>0</v>
       </c>
-      <c r="T17" s="20" t="s">
-        <v>197</v>
+      <c r="T17" s="19" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="18" spans="1:50">
@@ -7221,7 +7179,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="17">
-        <v>3902</v>
+        <v>2832</v>
       </c>
       <c r="R18" s="18">
         <f>iferror(lookup(if(Q18="",H18,Q18),{0,1,10,25,50,100,250,500},{0.0,0.29,0.271,0.2324,0.1974,0.1896,0.17028,0.16254}),"")</f>
@@ -7231,8 +7189,8 @@
         <f>iferror(if(Q18="",H18,Q18)*R18,"")</f>
         <v>0</v>
       </c>
-      <c r="T18" s="20" t="s">
-        <v>198</v>
+      <c r="T18" s="19" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:50">
@@ -7266,8 +7224,8 @@
         <f>iferror(H19*I19,"")</f>
         <v>0</v>
       </c>
-      <c r="P19" s="19" t="s">
-        <v>187</v>
+      <c r="P19" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R19" s="18">
         <f>iferror(lookup(if(Q19="",H19,Q19),{0,1,4000},{0.0,0.05769,0.05769}),"")</f>
@@ -7277,11 +7235,11 @@
         <f>iferror(if(Q19="",H19,Q19)*R19,"")</f>
         <v>0</v>
       </c>
-      <c r="T19" s="20" t="s">
-        <v>199</v>
-      </c>
-      <c r="U19" s="19" t="s">
-        <v>187</v>
+      <c r="T19" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="U19" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W19" s="18">
         <f>iferror(USD_GBP*lookup(if(V19="",H19,V19),{0,1,5,10,100,500,1000,5000},{0.0,0.29,0.29,0.196,0.0778,0.0585,0.0391,0.0332}),"")</f>
@@ -7291,8 +7249,8 @@
         <f>iferror(if(V19="",H19,V19)*W19,"")</f>
         <v>0</v>
       </c>
-      <c r="Y19" s="20" t="s">
-        <v>227</v>
+      <c r="Y19" s="19" t="s">
+        <v>228</v>
       </c>
       <c r="AE19" s="17">
         <v>2579</v>
@@ -7305,11 +7263,11 @@
         <f>iferror(if(AF19="",H19,AF19)*AG19,"")</f>
         <v>0</v>
       </c>
-      <c r="AI19" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="AJ19" s="19" t="s">
-        <v>187</v>
+      <c r="AI19" s="19" t="s">
+        <v>263</v>
+      </c>
+      <c r="AJ19" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL19" s="18">
         <f>iferror(lookup(if(AK19="",H19,AK19),{0,1,5,10,100,500,1000},{0.0,0.39,0.39,0.268,0.112,0.094,0.076}),"")</f>
@@ -7319,11 +7277,11 @@
         <f>iferror(if(AK19="",H19,AK19)*AL19,"")</f>
         <v>0</v>
       </c>
-      <c r="AN19" s="20" t="s">
-        <v>290</v>
-      </c>
-      <c r="AT19" s="19" t="s">
-        <v>187</v>
+      <c r="AN19" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="AT19" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AV19" s="18">
         <f>iferror(USD_GBP*lookup(if(AU19="",H19,AU19),{0,1,10,50,250,1000,4000},{0.0,0.06134,0.06134,0.04436,0.03994,0.03526,0.02963}),"")</f>
@@ -7333,7 +7291,7 @@
         <f>iferror(if(AU19="",H19,AU19)*AV19,"")</f>
         <v>0</v>
       </c>
-      <c r="AX19" s="20" t="s">
+      <c r="AX19" s="19" t="s">
         <v>318</v>
       </c>
     </row>
@@ -7368,8 +7326,8 @@
         <f>iferror(H20*I20,"")</f>
         <v>0</v>
       </c>
-      <c r="P20" s="19" t="s">
-        <v>187</v>
+      <c r="P20" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R20" s="18">
         <f>iferror(lookup(if(Q20="",H20,Q20),{0,1,10000},{0.0,0.0302,0.0302}),"")</f>
@@ -7379,8 +7337,8 @@
         <f>iferror(if(Q20="",H20,Q20)*R20,"")</f>
         <v>0</v>
       </c>
-      <c r="T20" s="20" t="s">
-        <v>200</v>
+      <c r="T20" s="19" t="s">
+        <v>201</v>
       </c>
       <c r="AE20" s="17">
         <v>10000</v>
@@ -7393,8 +7351,8 @@
         <f>iferror(if(AF20="",H20,AF20)*AG20,"")</f>
         <v>0</v>
       </c>
-      <c r="AI20" s="20" t="s">
-        <v>263</v>
+      <c r="AI20" s="19" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:50">
@@ -7429,7 +7387,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="17">
-        <v>4340071</v>
+        <v>6587632</v>
       </c>
       <c r="R21" s="18">
         <f>iferror(lookup(if(Q21="",H21,Q21),{0,1,10,25,50,100,250,500,1000,5000,15000,30000,75000},{0.0,0.1,0.025,0.018,0.0136,0.01,0.00764,0.00612,0.0045,0.00323,0.00281,0.00247,0.00231}),"")</f>
@@ -7439,11 +7397,11 @@
         <f>iferror(if(Q21="",H21,Q21)*R21,"")</f>
         <v>0</v>
       </c>
-      <c r="T21" s="20" t="s">
-        <v>201</v>
+      <c r="T21" s="19" t="s">
+        <v>202</v>
       </c>
       <c r="U21" s="17">
-        <v>95971</v>
+        <v>74971</v>
       </c>
       <c r="W21" s="18">
         <f>iferror(USD_GBP*lookup(if(V21="",H21,V21),{0,1,10,100,150,500,2500,7500,15000,75000},{0.0,0.04,0.04,0.024,0.024,0.018,0.012,0.009,0.007,0.0046}),"")</f>
@@ -7453,11 +7411,11 @@
         <f>iferror(if(V21="",H21,V21)*W21,"")</f>
         <v>0</v>
       </c>
-      <c r="Y21" s="20" t="s">
-        <v>228</v>
+      <c r="Y21" s="19" t="s">
+        <v>229</v>
       </c>
       <c r="AE21" s="17">
-        <v>894751</v>
+        <v>758499</v>
       </c>
       <c r="AG21" s="18">
         <f>iferror(lookup(if(AF21="",H21,AF21),{0,1,10,50,100,1000,10000},{0.0,0.1,0.014,0.014,0.006,0.005,0.003}),"")</f>
@@ -7467,11 +7425,11 @@
         <f>iferror(if(AF21="",H21,AF21)*AG21,"")</f>
         <v>0</v>
       </c>
-      <c r="AI21" s="20" t="s">
-        <v>264</v>
+      <c r="AI21" s="19" t="s">
+        <v>265</v>
       </c>
       <c r="AJ21" s="17">
-        <v>95971</v>
+        <v>65971</v>
       </c>
       <c r="AL21" s="18">
         <f>iferror(lookup(if(AK21="",H21,AK21),{0,1,25,100,250,500,1000,2500,5000,15000},{0.0,0.211,0.021,0.009,0.008,0.007,0.006,0.005,0.004,0.006}),"")</f>
@@ -7481,8 +7439,8 @@
         <f>iferror(if(AK21="",H21,AK21)*AL21,"")</f>
         <v>0</v>
       </c>
-      <c r="AN21" s="20" t="s">
-        <v>291</v>
+      <c r="AN21" s="19" t="s">
+        <v>292</v>
       </c>
       <c r="AO21" s="17">
         <v>1038637</v>
@@ -7495,8 +7453,8 @@
         <f>iferror(if(AP21="",H21,AP21)*AQ21,"")</f>
         <v>0</v>
       </c>
-      <c r="AS21" s="20" t="s">
-        <v>308</v>
+      <c r="AS21" s="19" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="22" spans="1:50">
@@ -7530,8 +7488,8 @@
         <f>iferror(H22*I22,"")</f>
         <v>0</v>
       </c>
-      <c r="P22" s="19" t="s">
-        <v>187</v>
+      <c r="P22" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R22" s="18">
         <f>iferror(lookup(if(Q22="",H22,Q22),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -7541,11 +7499,11 @@
         <f>iferror(if(Q22="",H22,Q22)*R22,"")</f>
         <v>0</v>
       </c>
-      <c r="T22" s="20" t="s">
-        <v>202</v>
-      </c>
-      <c r="U22" s="19" t="s">
-        <v>187</v>
+      <c r="T22" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="U22" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W22" s="18">
         <f>iferror(USD_GBP*lookup(if(V22="",H22,V22),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -7555,11 +7513,11 @@
         <f>iferror(if(V22="",H22,V22)*W22,"")</f>
         <v>0</v>
       </c>
-      <c r="Y22" s="20" t="s">
-        <v>229</v>
+      <c r="Y22" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="AE22" s="17">
-        <v>11274</v>
+        <v>6544</v>
       </c>
       <c r="AG22" s="18">
         <f>iferror(lookup(if(AF22="",H22,AF22),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.014,0.007,0.005}),"")</f>
@@ -7569,11 +7527,11 @@
         <f>iferror(if(AF22="",H22,AF22)*AG22,"")</f>
         <v>0</v>
       </c>
-      <c r="AI22" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="AJ22" s="19" t="s">
-        <v>187</v>
+      <c r="AI22" s="19" t="s">
+        <v>266</v>
+      </c>
+      <c r="AJ22" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL22" s="18">
         <f>iferror(lookup(if(AK22="",H22,AK22),{0,1,15000},{0.0,0.006,0.006}),"")</f>
@@ -7583,8 +7541,8 @@
         <f>iferror(if(AK22="",H22,AK22)*AL22,"")</f>
         <v>0</v>
       </c>
-      <c r="AN22" s="20" t="s">
-        <v>292</v>
+      <c r="AN22" s="19" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="1:50">
@@ -7618,8 +7576,8 @@
         <f>iferror(H23*I23,"")</f>
         <v>0</v>
       </c>
-      <c r="P23" s="19" t="s">
-        <v>187</v>
+      <c r="P23" s="17">
+        <v>133527</v>
       </c>
       <c r="R23" s="18">
         <f>iferror(lookup(if(Q23="",H23,Q23),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -7629,11 +7587,11 @@
         <f>iferror(if(Q23="",H23,Q23)*R23,"")</f>
         <v>0</v>
       </c>
-      <c r="T23" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="U23" s="19" t="s">
-        <v>187</v>
+      <c r="T23" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="U23" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W23" s="18">
         <f>iferror(USD_GBP*lookup(if(V23="",H23,V23),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -7643,25 +7601,25 @@
         <f>iferror(if(V23="",H23,V23)*W23,"")</f>
         <v>0</v>
       </c>
-      <c r="Y23" s="20" t="s">
-        <v>230</v>
+      <c r="Y23" s="19" t="s">
+        <v>231</v>
       </c>
       <c r="AE23" s="17">
-        <v>13882</v>
+        <v>26231</v>
       </c>
       <c r="AG23" s="18">
-        <f>iferror(lookup(if(AF23="",H23,AF23),{0,1,10,50,100,1000,10000},{0.0,0.1,0.025,0.025,0.008,0.005,0.003}),"")</f>
+        <f>iferror(lookup(if(AF23="",H23,AF23),{0,1,10,50,100,1000,10000},{0.0,0.1,0.031,0.031,0.014,0.007,0.005}),"")</f>
         <v>0</v>
       </c>
       <c r="AH23" s="18">
         <f>iferror(if(AF23="",H23,AF23)*AG23,"")</f>
         <v>0</v>
       </c>
-      <c r="AI23" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="AJ23" s="19" t="s">
-        <v>187</v>
+      <c r="AI23" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="AJ23" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL23" s="18">
         <f>iferror(lookup(if(AK23="",H23,AK23),{0,1,15000,30000},{0.0,0.005,0.005,0.004}),"")</f>
@@ -7671,8 +7629,8 @@
         <f>iferror(if(AK23="",H23,AK23)*AL23,"")</f>
         <v>0</v>
       </c>
-      <c r="AN23" s="20" t="s">
-        <v>293</v>
+      <c r="AN23" s="19" t="s">
+        <v>294</v>
       </c>
       <c r="AO23" s="17">
         <v>38000</v>
@@ -7685,8 +7643,8 @@
         <f>iferror(if(AP23="",H23,AP23)*AQ23,"")</f>
         <v>0</v>
       </c>
-      <c r="AS23" s="20" t="s">
-        <v>309</v>
+      <c r="AS23" s="19" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:50">
@@ -7721,7 +7679,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="17">
-        <v>491082</v>
+        <v>3137</v>
       </c>
       <c r="R24" s="18">
         <f>iferror(lookup(if(Q24="",H24,Q24),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -7731,11 +7689,11 @@
         <f>iferror(if(Q24="",H24,Q24)*R24,"")</f>
         <v>0</v>
       </c>
-      <c r="T24" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="U24" s="19" t="s">
-        <v>187</v>
+      <c r="T24" s="19" t="s">
+        <v>205</v>
+      </c>
+      <c r="U24" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W24" s="18">
         <f>iferror(USD_GBP*lookup(if(V24="",H24,V24),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -7745,11 +7703,11 @@
         <f>iferror(if(V24="",H24,V24)*W24,"")</f>
         <v>0</v>
       </c>
-      <c r="Y24" s="20" t="s">
-        <v>231</v>
+      <c r="Y24" s="19" t="s">
+        <v>232</v>
       </c>
       <c r="Z24" s="17">
-        <v>4000</v>
+        <v>3500</v>
       </c>
       <c r="AB24" s="18">
         <f>iferror(lookup(if(AA24="",H24,AA24),{0,1,50,500,1500,5000,25000,50000},{0.0,0.0197,0.0197,0.0151,0.0143,0.0135,0.0131,0.0129}),"")</f>
@@ -7759,25 +7717,25 @@
         <f>iferror(if(AA24="",H24,AA24)*AB24,"")</f>
         <v>0</v>
       </c>
-      <c r="AD24" s="20" t="s">
-        <v>248</v>
+      <c r="AD24" s="19" t="s">
+        <v>249</v>
       </c>
       <c r="AE24" s="17">
-        <v>80383</v>
+        <v>109423</v>
       </c>
       <c r="AG24" s="18">
-        <f>iferror(lookup(if(AF24="",H24,AF24),{0,1,10,50,100,1000,10000},{0.0,0.1,0.027,0.027,0.011,0.005,0.003}),"")</f>
+        <f>iferror(lookup(if(AF24="",H24,AF24),{0,1,10,50,100,1000,10000},{0.0,0.1,0.028,0.028,0.012,0.006,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AH24" s="18">
         <f>iferror(if(AF24="",H24,AF24)*AG24,"")</f>
         <v>0</v>
       </c>
-      <c r="AI24" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="AJ24" s="19" t="s">
-        <v>187</v>
+      <c r="AI24" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="AJ24" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL24" s="18">
         <f>iferror(lookup(if(AK24="",H24,AK24),{0,1,45000},{0.0,0.004,0.004}),"")</f>
@@ -7787,22 +7745,8 @@
         <f>iferror(if(AK24="",H24,AK24)*AL24,"")</f>
         <v>0</v>
       </c>
-      <c r="AN24" s="20" t="s">
-        <v>294</v>
-      </c>
-      <c r="AO24" s="17">
-        <v>8000</v>
-      </c>
-      <c r="AQ24" s="18">
-        <f>iferror(USD_GBP*lookup(if(AP24="",H24,AP24),{0,1,15000},{0.0,0.006,0.006}),"")</f>
-        <v>0</v>
-      </c>
-      <c r="AR24" s="18">
-        <f>iferror(if(AP24="",H24,AP24)*AQ24,"")</f>
-        <v>0</v>
-      </c>
-      <c r="AS24" s="20" t="s">
-        <v>310</v>
+      <c r="AN24" s="19" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:50">
@@ -7837,7 +7781,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="17">
-        <v>70771</v>
+        <v>70750</v>
       </c>
       <c r="R25" s="18">
         <f>iferror(lookup(if(Q25="",H25,Q25),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -7847,11 +7791,11 @@
         <f>iferror(if(Q25="",H25,Q25)*R25,"")</f>
         <v>0</v>
       </c>
-      <c r="T25" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="U25" s="19" t="s">
-        <v>187</v>
+      <c r="T25" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="U25" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W25" s="18">
         <f>iferror(USD_GBP*lookup(if(V25="",H25,V25),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -7861,8 +7805,8 @@
         <f>iferror(if(V25="",H25,V25)*W25,"")</f>
         <v>0</v>
       </c>
-      <c r="Y25" s="20" t="s">
-        <v>232</v>
+      <c r="Y25" s="19" t="s">
+        <v>233</v>
       </c>
       <c r="AE25" s="17">
         <v>80525</v>
@@ -7875,14 +7819,14 @@
         <f>iferror(if(AF25="",H25,AF25)*AG25,"")</f>
         <v>0</v>
       </c>
-      <c r="AI25" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="AJ25" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="AN25" s="20" t="s">
-        <v>295</v>
+      <c r="AI25" s="19" t="s">
+        <v>269</v>
+      </c>
+      <c r="AJ25" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="AN25" s="19" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="26" spans="1:50">
@@ -7917,7 +7861,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="17">
-        <v>13201</v>
+        <v>11996</v>
       </c>
       <c r="R26" s="18">
         <f>iferror(lookup(if(Q26="",H26,Q26),{0,1,10,100,1000,2500,5000,15000},{0.0,0.1,0.028,0.0115,0.00518,0.0045,0.00371,0.00323}),"")</f>
@@ -7927,11 +7871,11 @@
         <f>iferror(if(Q26="",H26,Q26)*R26,"")</f>
         <v>0</v>
       </c>
-      <c r="T26" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="U26" s="19" t="s">
-        <v>187</v>
+      <c r="T26" s="19" t="s">
+        <v>207</v>
+      </c>
+      <c r="U26" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W26" s="18">
         <f>iferror(USD_GBP*lookup(if(V26="",H26,V26),{0,1,30000},{0.0,0.0046,0.0046}),"")</f>
@@ -7941,8 +7885,8 @@
         <f>iferror(if(V26="",H26,V26)*W26,"")</f>
         <v>0</v>
       </c>
-      <c r="Y26" s="20" t="s">
-        <v>233</v>
+      <c r="Y26" s="19" t="s">
+        <v>234</v>
       </c>
       <c r="Z26" s="17">
         <v>14800</v>
@@ -7955,28 +7899,28 @@
         <f>iferror(if(AA26="",H26,AA26)*AB26,"")</f>
         <v>0</v>
       </c>
-      <c r="AD26" s="20" t="s">
-        <v>249</v>
+      <c r="AD26" s="19" t="s">
+        <v>250</v>
       </c>
       <c r="AE26" s="17">
-        <v>87234</v>
+        <v>145444</v>
       </c>
       <c r="AG26" s="18">
-        <f>iferror(lookup(if(AF26="",H26,AF26),{0,1,10,50,100,1000,10000},{0.0,0.1,0.027,0.027,0.011,0.005,0.003}),"")</f>
+        <f>iferror(lookup(if(AF26="",H26,AF26),{0,1,10,50,100,1000,10000},{0.0,0.1,0.028,0.028,0.012,0.006,0.003}),"")</f>
         <v>0</v>
       </c>
       <c r="AH26" s="18">
         <f>iferror(if(AF26="",H26,AF26)*AG26,"")</f>
         <v>0</v>
       </c>
-      <c r="AI26" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="AJ26" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="AN26" s="20" t="s">
-        <v>296</v>
+      <c r="AI26" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="AJ26" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="AN26" s="19" t="s">
+        <v>297</v>
       </c>
       <c r="AO26" s="17">
         <v>37000</v>
@@ -7989,7 +7933,7 @@
         <f>iferror(if(AP26="",H26,AP26)*AQ26,"")</f>
         <v>0</v>
       </c>
-      <c r="AS26" s="20" t="s">
+      <c r="AS26" s="19" t="s">
         <v>311</v>
       </c>
     </row>
@@ -8028,18 +7972,18 @@
         <v>1191</v>
       </c>
       <c r="R27" s="18">
-        <f>iferror(lookup(if(Q27="",H27,Q27),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000,75000},{0.0,0.35,0.258,0.2256,0.146,0.12084,0.09668,0.07412,0.06445,0.058,0.05156,0.04834,0.0456}),"")</f>
+        <f>iferror(lookup(if(Q27="",H27,Q27),{0,1,10,25,100,250,500,1000,3000,6000,15000},{0.0,0.46,0.343,0.3004,0.1945,0.161,0.1288,0.09874,0.08586,0.07727,0.07087}),"")</f>
         <v>0</v>
       </c>
       <c r="S27" s="18">
         <f>iferror(if(Q27="",H27,Q27)*R27,"")</f>
         <v>0</v>
       </c>
-      <c r="T27" s="20" t="s">
-        <v>207</v>
+      <c r="T27" s="19" t="s">
+        <v>208</v>
       </c>
       <c r="U27" s="17">
-        <v>1973</v>
+        <v>1972</v>
       </c>
       <c r="W27" s="18">
         <f>iferror(USD_GBP*lookup(if(V27="",H27,V27),{0,1,5,10,100,500,3000},{0.0,0.334,0.334,0.224,0.0886,0.0551,0.0434}),"")</f>
@@ -8049,11 +7993,11 @@
         <f>iferror(if(V27="",H27,V27)*W27,"")</f>
         <v>0</v>
       </c>
-      <c r="Y27" s="20" t="s">
-        <v>234</v>
+      <c r="Y27" s="19" t="s">
+        <v>235</v>
       </c>
       <c r="AE27" s="17">
-        <v>13244</v>
+        <v>13241</v>
       </c>
       <c r="AG27" s="18">
         <f>iferror(lookup(if(AF27="",H27,AF27),{0,1,10,50,100,1000,10000},{0.0,0.46,0.343,0.343,0.172,0.099,0.068}),"")</f>
@@ -8063,22 +8007,22 @@
         <f>iferror(if(AF27="",H27,AF27)*AG27,"")</f>
         <v>0</v>
       </c>
-      <c r="AI27" s="20" t="s">
-        <v>270</v>
+      <c r="AI27" s="19" t="s">
+        <v>271</v>
       </c>
       <c r="AJ27" s="17">
-        <v>1948</v>
+        <v>1947</v>
       </c>
       <c r="AL27" s="18">
-        <f>iferror(lookup(if(AK27="",H27,AK27),{0,1,5,10,25,50,100,250,500,1000,3000,12000,18000,48000,90000},{0.0,0.312,0.312,0.24,0.164,0.136,0.114,0.091,0.076,0.063,0.05,0.05,0.042,0.038,0.036}),"")</f>
+        <f>iferror(lookup(if(AK27="",H27,AK27),{0,1,5,10,100,6000,9000,24000,45000},{0.0,0.363,0.363,0.296,0.138,0.059,0.055,0.051,0.048}),"")</f>
         <v>0</v>
       </c>
       <c r="AM27" s="18">
         <f>iferror(if(AK27="",H27,AK27)*AL27,"")</f>
         <v>0</v>
       </c>
-      <c r="AN27" s="20" t="s">
-        <v>297</v>
+      <c r="AN27" s="19" t="s">
+        <v>298</v>
       </c>
       <c r="AO27" s="17">
         <v>3000</v>
@@ -8091,7 +8035,7 @@
         <f>iferror(if(AP27="",H27,AP27)*AQ27,"")</f>
         <v>0</v>
       </c>
-      <c r="AS27" s="20" t="s">
+      <c r="AS27" s="19" t="s">
         <v>312</v>
       </c>
     </row>
@@ -8126,8 +8070,8 @@
         <f>iferror(H28*I28,"")</f>
         <v>0</v>
       </c>
-      <c r="P28" s="19" t="s">
-        <v>187</v>
+      <c r="P28" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R28" s="18">
         <f>iferror(lookup(if(Q28="",H28,Q28),{0,1,2000},{0.0,1.336,1.336}),"")</f>
@@ -8137,8 +8081,8 @@
         <f>iferror(if(Q28="",H28,Q28)*R28,"")</f>
         <v>0</v>
       </c>
-      <c r="T28" s="20" t="s">
-        <v>208</v>
+      <c r="T28" s="19" t="s">
+        <v>209</v>
       </c>
       <c r="Z28" s="17">
         <v>1990</v>
@@ -8151,8 +8095,8 @@
         <f>iferror(if(AA28="",H28,AA28)*AB28,"")</f>
         <v>0</v>
       </c>
-      <c r="AD28" s="20" t="s">
-        <v>250</v>
+      <c r="AD28" s="19" t="s">
+        <v>251</v>
       </c>
       <c r="AE28" s="17">
         <v>594</v>
@@ -8165,8 +8109,8 @@
         <f>iferror(if(AF28="",H28,AF28)*AG28,"")</f>
         <v>0</v>
       </c>
-      <c r="AI28" s="20" t="s">
-        <v>271</v>
+      <c r="AI28" s="19" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="29" spans="1:50">
@@ -8211,8 +8155,8 @@
         <f>iferror(if(Q29="",H29,Q29)*R29,"")</f>
         <v>0</v>
       </c>
-      <c r="T29" s="20" t="s">
-        <v>209</v>
+      <c r="T29" s="19" t="s">
+        <v>210</v>
       </c>
       <c r="U29" s="17">
         <v>2706</v>
@@ -8225,11 +8169,11 @@
         <f>iferror(if(V29="",H29,V29)*W29,"")</f>
         <v>0</v>
       </c>
-      <c r="Y29" s="20" t="s">
-        <v>235</v>
+      <c r="Y29" s="19" t="s">
+        <v>236</v>
       </c>
       <c r="AE29" s="17">
-        <v>2522</v>
+        <v>2519</v>
       </c>
       <c r="AG29" s="18">
         <f>iferror(lookup(if(AF29="",H29,AF29),{0,1,10,50,100,1000,10000},{0.0,0.61,0.518,0.518,0.359,0.235,0.188}),"")</f>
@@ -8239,8 +8183,8 @@
         <f>iferror(if(AF29="",H29,AF29)*AG29,"")</f>
         <v>0</v>
       </c>
-      <c r="AI29" s="20" t="s">
-        <v>272</v>
+      <c r="AI29" s="19" t="s">
+        <v>273</v>
       </c>
       <c r="AJ29" s="17">
         <v>2706</v>
@@ -8253,8 +8197,8 @@
         <f>iferror(if(AK29="",H29,AK29)*AL29,"")</f>
         <v>0</v>
       </c>
-      <c r="AN29" s="20" t="s">
-        <v>298</v>
+      <c r="AN29" s="19" t="s">
+        <v>299</v>
       </c>
       <c r="AO29" s="17">
         <v>100</v>
@@ -8267,11 +8211,11 @@
         <f>iferror(if(AP29="",H29,AP29)*AQ29,"")</f>
         <v>0</v>
       </c>
-      <c r="AS29" s="20" t="s">
+      <c r="AS29" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="AT29" s="19" t="s">
-        <v>187</v>
+      <c r="AT29" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AV29" s="18">
         <f>iferror(USD_GBP*lookup(if(AU29="",H29,AU29),{0,1,3,25,100,250,1000},{0.0,0.20481,0.20481,0.17389,0.15457,0.14491,0.13525}),"")</f>
@@ -8281,7 +8225,7 @@
         <f>iferror(if(AU29="",H29,AU29)*AV29,"")</f>
         <v>0</v>
       </c>
-      <c r="AX29" s="20" t="s">
+      <c r="AX29" s="19" t="s">
         <v>123</v>
       </c>
     </row>
@@ -8316,36 +8260,36 @@
         <f>iferror(H30*I30,"")</f>
         <v>0</v>
       </c>
-      <c r="P30" s="17">
-        <v>2741</v>
+      <c r="P30" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R30" s="18">
-        <f>iferror(lookup(if(Q30="",H30,Q30),{0,1,10,25,100,250,500,1000,3000,6000,15000,30000},{0.0,0.54,0.438,0.4012,0.2985,0.27052,0.22388,0.1679,0.15391,0.14458,0.13526,0.132}),"")</f>
+        <f>iferror(lookup(if(Q30="",H30,Q30),{0,1,10,25,100,250,500,1000,3000},{0.0,0.47,0.402,0.3756,0.3004,0.27892,0.236,0.18236,0.1771}),"")</f>
         <v>0</v>
       </c>
       <c r="S30" s="18">
         <f>iferror(if(Q30="",H30,Q30)*R30,"")</f>
         <v>0</v>
       </c>
-      <c r="T30" s="20" t="s">
-        <v>210</v>
+      <c r="T30" s="19" t="s">
+        <v>211</v>
       </c>
       <c r="U30" s="17">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="W30" s="18">
-        <f>iferror(USD_GBP*lookup(if(V30="",H30,V30),{0,1,5,10,100,150,500,3000,9000,24000,45000},{0.0,0.422,0.422,0.309,0.142,0.142,0.105,0.0914,0.0882,0.0851,0.0836}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V30="",H30,V30),{0,1,5,10,100,150,500,3000},{0.0,0.589,0.589,0.428,0.214,0.214,0.146,0.133}),"")</f>
         <v>0</v>
       </c>
       <c r="X30" s="18">
         <f>iferror(if(V30="",H30,V30)*W30,"")</f>
         <v>0</v>
       </c>
-      <c r="Y30" s="20" t="s">
-        <v>236</v>
+      <c r="Y30" s="19" t="s">
+        <v>237</v>
       </c>
       <c r="AE30" s="17">
-        <v>8389</v>
+        <v>7289</v>
       </c>
       <c r="AG30" s="18">
         <f>iferror(lookup(if(AF30="",H30,AF30),{0,1,10,50,100,1000,10000},{0.0,0.47,0.403,0.403,0.279,0.183,0.146}),"")</f>
@@ -8355,22 +8299,22 @@
         <f>iferror(if(AF30="",H30,AF30)*AG30,"")</f>
         <v>0</v>
       </c>
-      <c r="AI30" s="20" t="s">
-        <v>273</v>
+      <c r="AI30" s="19" t="s">
+        <v>274</v>
       </c>
       <c r="AJ30" s="17">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="AL30" s="18">
-        <f>iferror(lookup(if(AK30="",H30,AK30),{0,1,5,10,25,50,100,250,500,1000,3000,6000,12000,18000,24000,30000,300000},{0.0,0.582,0.582,0.447,0.372,0.313,0.262,0.223,0.182,0.155,0.141,0.132,0.121,0.121,0.12,0.12,0.12}),"")</f>
+        <f>iferror(lookup(if(AK30="",H30,AK30),{0,1,5,10,100,3000,6000,12000,18000,24000,30000,300000},{0.0,0.613,0.613,0.455,0.233,0.138,0.136,0.134,0.132,0.13,0.129,0.127}),"")</f>
         <v>0</v>
       </c>
       <c r="AM30" s="18">
         <f>iferror(if(AK30="",H30,AK30)*AL30,"")</f>
         <v>0</v>
       </c>
-      <c r="AN30" s="20" t="s">
-        <v>299</v>
+      <c r="AN30" s="19" t="s">
+        <v>300</v>
       </c>
       <c r="AO30" s="17">
         <v>12</v>
@@ -8383,7 +8327,7 @@
         <f>iferror(if(AP30="",H30,AP30)*AQ30,"")</f>
         <v>0</v>
       </c>
-      <c r="AS30" s="20" t="s">
+      <c r="AS30" s="19" t="s">
         <v>314</v>
       </c>
     </row>
@@ -8418,8 +8362,8 @@
         <f>iferror(H31*I31,"")</f>
         <v>0</v>
       </c>
-      <c r="P31" s="19" t="s">
-        <v>187</v>
+      <c r="P31" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R31" s="18">
         <f>iferror(lookup(if(Q31="",H31,Q31),{0,1,5000},{0.0,0.22138,0.22138}),"")</f>
@@ -8429,11 +8373,11 @@
         <f>iferror(if(Q31="",H31,Q31)*R31,"")</f>
         <v>0</v>
       </c>
-      <c r="T31" s="20" t="s">
-        <v>211</v>
-      </c>
-      <c r="U31" s="19" t="s">
-        <v>187</v>
+      <c r="T31" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="U31" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W31" s="18">
         <f>iferror(USD_GBP*lookup(if(V31="",H31,V31),{0,1,5000},{0.0,0.126,0.126}),"")</f>
@@ -8443,8 +8387,8 @@
         <f>iferror(if(V31="",H31,V31)*W31,"")</f>
         <v>0</v>
       </c>
-      <c r="Y31" s="20" t="s">
-        <v>237</v>
+      <c r="Y31" s="19" t="s">
+        <v>238</v>
       </c>
       <c r="AE31" s="17">
         <v>3515</v>
@@ -8457,8 +8401,8 @@
         <f>iferror(if(AF31="",H31,AF31)*AG31,"")</f>
         <v>0</v>
       </c>
-      <c r="AI31" s="20" t="s">
-        <v>274</v>
+      <c r="AI31" s="19" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="32" spans="1:50">
@@ -8472,7 +8416,7 @@
         <v>135</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>136</v>
@@ -8481,7 +8425,7 @@
         <v>137</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="H32" s="17">
         <f>BoardQty*1</f>
@@ -8495,81 +8439,81 @@
         <f>iferror(H32*I32,"")</f>
         <v>0</v>
       </c>
-      <c r="P32" s="19" t="s">
-        <v>187</v>
+      <c r="P32" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R32" s="18">
-        <f>iferror(lookup(if(Q32="",H32,Q32),{0,1,10},{0.0,3.54,3.5}),"")</f>
+        <f>iferror(lookup(if(Q32="",H32,Q32),{0,1,5000},{0.0,3.63,3.49965}),"")</f>
         <v>0</v>
       </c>
       <c r="S32" s="18">
         <f>iferror(if(Q32="",H32,Q32)*R32,"")</f>
         <v>0</v>
       </c>
-      <c r="T32" s="20" t="s">
-        <v>212</v>
-      </c>
-      <c r="U32" s="19" t="s">
-        <v>187</v>
+      <c r="T32" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="U32" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W32" s="18">
-        <f>iferror(USD_GBP*lookup(if(V32="",H32,V32),{0,1,10,25,50,100,250,500,1000},{0.0,2.9,2.17,2.05,1.92,1.8,1.61,1.54,1.28}),"")</f>
+        <f>iferror(USD_GBP*lookup(if(V32="",H32,V32),{0,1,10,25,50,100},{0.0,3.61,2.74,2.69,2.64,2.59}),"")</f>
         <v>0</v>
       </c>
       <c r="X32" s="18">
         <f>iferror(if(V32="",H32,V32)*W32,"")</f>
         <v>0</v>
       </c>
-      <c r="Y32" s="20" t="s">
-        <v>238</v>
-      </c>
-      <c r="AE32" s="19" t="s">
-        <v>187</v>
+      <c r="Y32" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="AE32" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG32" s="18">
-        <f>iferror(lookup(if(AF32="",H32,AF32),{0,1,10,50,100,1000,10000},{0.0,3.58,3.22,3.04,2.64,2.55,2.54}),"")</f>
+        <f>iferror(lookup(if(AF32="",H32,AF32),{0,1,10,50,100,1000,10000},{0.0,3.58,3.22,3.04,2.64,2.59,2.54}),"")</f>
         <v>0</v>
       </c>
       <c r="AH32" s="18">
         <f>iferror(if(AF32="",H32,AF32)*AG32,"")</f>
         <v>0</v>
       </c>
-      <c r="AI32" s="20" t="s">
-        <v>275</v>
-      </c>
-      <c r="AJ32" s="19" t="s">
-        <v>187</v>
+      <c r="AI32" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ32" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL32" s="18">
-        <f>iferror(lookup(if(AK32="",H32,AK32),{0,1,10,25,50,100,250,2450},{0.0,3.83,3.13,2.94,2.76,2.58,2.31,2.31}),"")</f>
+        <f>iferror(lookup(if(AK32="",H32,AK32),{0,1,5000},{0.0,3.45,3.33}),"")</f>
         <v>0</v>
       </c>
       <c r="AM32" s="18">
         <f>iferror(if(AK32="",H32,AK32)*AL32,"")</f>
         <v>0</v>
       </c>
-      <c r="AN32" s="20" t="s">
-        <v>300</v>
+      <c r="AN32" s="19" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:50">
       <c r="A33" s="17" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C33" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="17" t="s">
         <v>141</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>142</v>
-      </c>
-      <c r="F33" s="17" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>140</v>
       </c>
       <c r="H33" s="17">
         <f>BoardQty*1</f>
@@ -8584,7 +8528,7 @@
         <v>0</v>
       </c>
       <c r="P33" s="17">
-        <v>280</v>
+        <v>233</v>
       </c>
       <c r="R33" s="18">
         <f>iferror(lookup(if(Q33="",H33,Q33),{0,1},{0.0,3.6}),"")</f>
@@ -8594,11 +8538,11 @@
         <f>iferror(if(Q33="",H33,Q33)*R33,"")</f>
         <v>0</v>
       </c>
-      <c r="T33" s="20" t="s">
-        <v>213</v>
-      </c>
-      <c r="AE33" s="19" t="s">
-        <v>187</v>
+      <c r="T33" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE33" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG33" s="18">
         <f>iferror(lookup(if(AF33="",H33,AF33),{0,1,10,50,100,1000,10000},{0.0,3.2,3.2,3.2,3.2,3.2,3.2}),"")</f>
@@ -8608,11 +8552,11 @@
         <f>iferror(if(AF33="",H33,AF33)*AG33,"")</f>
         <v>0</v>
       </c>
-      <c r="AI33" s="20" t="s">
-        <v>276</v>
-      </c>
-      <c r="AT33" s="19" t="s">
-        <v>187</v>
+      <c r="AI33" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="AT33" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AV33" s="18">
         <f>iferror(USD_GBP*lookup(if(AU33="",H33,AU33),{0,1,5,25,100},{0.0,2.98,2.8,2.62,2.44}),"")</f>
@@ -8622,28 +8566,28 @@
         <f>iferror(if(AU33="",H33,AU33)*AV33,"")</f>
         <v>0</v>
       </c>
-      <c r="AX33" s="20" t="s">
+      <c r="AX33" s="19" t="s">
         <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:50">
       <c r="A34" s="17" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="C34" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H34" s="17">
         <f>BoardQty*1</f>
@@ -8657,8 +8601,8 @@
         <f>iferror(H34*I34,"")</f>
         <v>0</v>
       </c>
-      <c r="P34" s="19" t="s">
-        <v>187</v>
+      <c r="P34" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="R34" s="18">
         <f>iferror(lookup(if(Q34="",H34,Q34),{0,1,1500},{0.0,1.41,1.41}),"")</f>
@@ -8668,11 +8612,11 @@
         <f>iferror(if(Q34="",H34,Q34)*R34,"")</f>
         <v>0</v>
       </c>
-      <c r="T34" s="20" t="s">
-        <v>214</v>
-      </c>
-      <c r="U34" s="19" t="s">
-        <v>187</v>
+      <c r="T34" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="U34" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="W34" s="18">
         <f>iferror(USD_GBP*lookup(if(V34="",H34,V34),{0,1,10,50,100,250},{0.0,1.46,1.24,1.22,1.19,1.17}),"")</f>
@@ -8682,11 +8626,11 @@
         <f>iferror(if(V34="",H34,V34)*W34,"")</f>
         <v>0</v>
       </c>
-      <c r="Y34" s="20" t="s">
-        <v>239</v>
-      </c>
-      <c r="AE34" s="19" t="s">
-        <v>187</v>
+      <c r="Y34" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="AE34" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AG34" s="18">
         <f>iferror(lookup(if(AF34="",H34,AF34),{0,1,10,50,100,1000,10000},{0.0,1.35,1.35,1.3,1.25,1.25,1.25}),"")</f>
@@ -8696,42 +8640,42 @@
         <f>iferror(if(AF34="",H34,AF34)*AG34,"")</f>
         <v>0</v>
       </c>
-      <c r="AI34" s="20" t="s">
-        <v>277</v>
-      </c>
-      <c r="AJ34" s="19" t="s">
-        <v>187</v>
+      <c r="AI34" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="AJ34" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL34" s="18">
-        <f>iferror(lookup(if(AK34="",H34,AK34),{0,1,10,25,50,100},{0.0,2.13,1.98,1.85,1.73,1.61}),"")</f>
+        <f>iferror(lookup(if(AK34="",H34,AK34),{0,1,10,25,50,100},{0.0,2.16,2.01,1.89,1.76,1.64}),"")</f>
         <v>0</v>
       </c>
       <c r="AM34" s="18">
         <f>iferror(if(AK34="",H34,AK34)*AL34,"")</f>
         <v>0</v>
       </c>
-      <c r="AN34" s="20" t="s">
-        <v>301</v>
+      <c r="AN34" s="19" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="35" spans="1:50">
       <c r="A35" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B35" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F35" s="17" t="s">
         <v>52</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H35" s="17">
         <f>BoardQty*1</f>
@@ -8756,14 +8700,14 @@
         <f>iferror(if(Q35="",H35,Q35)*R35,"")</f>
         <v>0</v>
       </c>
-      <c r="T35" s="20" t="s">
-        <v>215</v>
-      </c>
-      <c r="U35" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="Y35" s="20" t="s">
-        <v>240</v>
+      <c r="T35" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="U35" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="Y35" s="19" t="s">
+        <v>241</v>
       </c>
       <c r="Z35" s="17">
         <v>2781</v>
@@ -8776,8 +8720,8 @@
         <f>iferror(if(AA35="",H35,AA35)*AB35,"")</f>
         <v>0</v>
       </c>
-      <c r="AD35" s="20" t="s">
-        <v>251</v>
+      <c r="AD35" s="19" t="s">
+        <v>252</v>
       </c>
       <c r="AE35" s="17">
         <v>5089</v>
@@ -8790,11 +8734,11 @@
         <f>iferror(if(AF35="",H35,AF35)*AG35,"")</f>
         <v>0</v>
       </c>
-      <c r="AI35" s="20" t="s">
-        <v>278</v>
-      </c>
-      <c r="AJ35" s="19" t="s">
-        <v>187</v>
+      <c r="AI35" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ35" s="20" t="s">
+        <v>189</v>
       </c>
       <c r="AL35" s="18">
         <f>iferror(lookup(if(AK35="",H35,AK35),{0,1,3000,9000,24000,45000},{0.0,0.225,0.225,0.219,0.212,0.206}),"")</f>
@@ -8804,28 +8748,28 @@
         <f>iferror(if(AK35="",H35,AK35)*AL35,"")</f>
         <v>0</v>
       </c>
-      <c r="AN35" s="20" t="s">
-        <v>302</v>
+      <c r="AN35" s="19" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="36" spans="1:50">
       <c r="A36" s="17" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B36" s="17" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C36" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="G36" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>157</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>155</v>
       </c>
       <c r="H36" s="17">
         <f>BoardQty*1</f>
@@ -8840,7 +8784,7 @@
         <v>0</v>
       </c>
       <c r="P36" s="17">
-        <v>333</v>
+        <v>1192</v>
       </c>
       <c r="R36" s="18">
         <f>iferror(lookup(if(Q36="",H36,Q36),{0,1,25,100,2000},{0.0,6.0,5.25,5.005,5.005}),"")</f>
@@ -8850,11 +8794,11 @@
         <f>iferror(if(Q36="",H36,Q36)*R36,"")</f>
         <v>0</v>
       </c>
-      <c r="T36" s="20" t="s">
-        <v>216</v>
+      <c r="T36" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="AE36" s="17">
-        <v>2559</v>
+        <v>470</v>
       </c>
       <c r="AG36" s="18">
         <f>iferror(lookup(if(AF36="",H36,AF36),{0,1,10,50,100,1000,10000},{0.0,6.06,6.06,5.31,5.06,5.06,5.05}),"")</f>
@@ -8864,31 +8808,31 @@
         <f>iferror(if(AF36="",H36,AF36)*AG36,"")</f>
         <v>0</v>
       </c>
-      <c r="AI36" s="20" t="s">
-        <v>279</v>
+      <c r="AI36" s="19" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="37" spans="1:50">
       <c r="A37" s="17" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B37" s="17" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C37" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="G37" s="17" t="s">
         <v>161</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>162</v>
-      </c>
-      <c r="F37" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="G37" s="17" t="s">
-        <v>160</v>
       </c>
       <c r="H37" s="17">
         <f>BoardQty*1</f>
@@ -8905,17 +8849,17 @@
     </row>
     <row r="39" spans="1:50">
       <c r="B39" s="21" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J39" s="5">
         <f>SUM(INDIRECT(ADDRESS(ROW(),COLUMN(arrow_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(digikey_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(farnell_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(mouser_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(newark_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(rs_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(tme_part_data)+3)),INDIRECT(ADDRESS(ROW(),COLUMN(lcsc_part_data)+3)))</f>
         <v>0</v>
       </c>
-      <c r="K39" s="20" t="s">
-        <v>184</v>
+      <c r="K39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="L39" s="6">
         <f>IFERROR(IF(OR(L7:L37),COUNTIFS(L7:L37,"&gt;0",N7:N37,"&lt;&gt;")&amp;" of "&amp;(ROWS(N7:N37)-COUNTBLANK(N7:N37))&amp;" parts purchased",""),"")</f>
@@ -8925,8 +8869,8 @@
         <f>SUMIF(L7:L37,"&gt;0",N7:N37)</f>
         <v>0</v>
       </c>
-      <c r="P39" s="20" t="s">
-        <v>184</v>
+      <c r="P39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="Q39" s="6">
         <f>IFERROR(IF(OR(Q7:Q37),COUNTIFS(Q7:Q37,"&gt;0",S7:S37,"&lt;&gt;")&amp;" of "&amp;(ROWS(S7:S37)-COUNTBLANK(S7:S37))&amp;" parts purchased",""),"")</f>
@@ -8936,8 +8880,8 @@
         <f>SUMIF(Q7:Q37,"&gt;0",S7:S37)</f>
         <v>0</v>
       </c>
-      <c r="U39" s="20" t="s">
-        <v>184</v>
+      <c r="U39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="V39" s="6">
         <f>IFERROR(IF(OR(V7:V37),COUNTIFS(V7:V37,"&gt;0",X7:X37,"&lt;&gt;")&amp;" of "&amp;(ROWS(X7:X37)-COUNTBLANK(X7:X37))&amp;" parts purchased",""),"")</f>
@@ -8947,8 +8891,8 @@
         <f>SUMIF(V7:V37,"&gt;0",X7:X37)</f>
         <v>0</v>
       </c>
-      <c r="Z39" s="20" t="s">
-        <v>184</v>
+      <c r="Z39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="AA39" s="6">
         <f>IFERROR(IF(OR(AA7:AA37),COUNTIFS(AA7:AA37,"&gt;0",AC7:AC37,"&lt;&gt;")&amp;" of "&amp;(ROWS(AC7:AC37)-COUNTBLANK(AC7:AC37))&amp;" parts purchased",""),"")</f>
@@ -8958,8 +8902,8 @@
         <f>SUMIF(AA7:AA37,"&gt;0",AC7:AC37)</f>
         <v>0</v>
       </c>
-      <c r="AE39" s="20" t="s">
-        <v>184</v>
+      <c r="AE39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="AF39" s="6">
         <f>IFERROR(IF(OR(AF7:AF37),COUNTIFS(AF7:AF37,"&gt;0",AH7:AH37,"&lt;&gt;")&amp;" of "&amp;(ROWS(AH7:AH37)-COUNTBLANK(AH7:AH37))&amp;" parts purchased",""),"")</f>
@@ -8969,8 +8913,8 @@
         <f>SUMIF(AF7:AF37,"&gt;0",AH7:AH37)</f>
         <v>0</v>
       </c>
-      <c r="AJ39" s="20" t="s">
-        <v>184</v>
+      <c r="AJ39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="AK39" s="6">
         <f>IFERROR(IF(OR(AK7:AK37),COUNTIFS(AK7:AK37,"&gt;0",AM7:AM37,"&lt;&gt;")&amp;" of "&amp;(ROWS(AM7:AM37)-COUNTBLANK(AM7:AM37))&amp;" parts purchased",""),"")</f>
@@ -8980,8 +8924,8 @@
         <f>SUMIF(AK7:AK37,"&gt;0",AM7:AM37)</f>
         <v>0</v>
       </c>
-      <c r="AO39" s="20" t="s">
-        <v>184</v>
+      <c r="AO39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="AP39" s="6">
         <f>IFERROR(IF(OR(AP7:AP37),COUNTIFS(AP7:AP37,"&gt;0",AR7:AR37,"&lt;&gt;")&amp;" of "&amp;(ROWS(AR7:AR37)-COUNTBLANK(AR7:AR37))&amp;" parts purchased",""),"")</f>
@@ -8991,8 +8935,8 @@
         <f>SUMIF(AP7:AP37,"&gt;0",AR7:AR37)</f>
         <v>0</v>
       </c>
-      <c r="AT39" s="20" t="s">
-        <v>184</v>
+      <c r="AT39" s="19" t="s">
+        <v>185</v>
       </c>
       <c r="AU39" s="6">
         <f>IFERROR(IF(OR(AU7:AU37),COUNTIFS(AU7:AU37,"&gt;0",AW7:AW37,"&lt;&gt;")&amp;" of "&amp;(ROWS(AW7:AW37)-COUNTBLANK(AW7:AW37))&amp;" parts purchased",""),"")</f>
@@ -9005,13 +8949,13 @@
     </row>
     <row r="40" spans="1:50">
       <c r="B40" s="21" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C40">
         <v>1.293904700565222</v>
       </c>
       <c r="I40" s="21" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="L40">
         <f t="array" ref="L40">IFERROR(CONCATENATE(INDEX(O7:O37,SMALL(IF(ISNUMBER(L7:L37),IF(L7:L37&gt;0,IF(O7:O37&lt;&gt;"",ROW(L7:L37)-MIN(ROW(L7:L37))+1))),ROW()-ROW(A$40)+1)),",",TEXT(INDEX(L7:L37,SMALL(IF(ISNUMBER(L7:L37),IF(L7:L37&gt;0,IF(O7:O37&lt;&gt;"",ROW(L7:L37)-MIN(ROW(L7:L37))+1))),ROW()-ROW(A$40)+1)),"##0"),",",SUBSTITUTE(INDEX(IF(PURCHASE_DESCRIPTION&lt;&gt;"",PURCHASE_DESCRIPTION&amp;":","")&amp;A7:A37,SMALL(IF(ISNUMBER(L7:L37),IF(L7:L37&gt;0,IF(O7:O37&lt;&gt;"",ROW(L7:L37)-MIN(ROW(L7:L37))+1))),ROW()-ROW(A$40)+1)),",",";")),"")</f>
@@ -11675,43 +11619,35 @@
       <formula>H23</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AO24">
+  <conditionalFormatting sqref="AO26">
     <cfRule type="cellIs" dxfId="1" priority="749" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="750" operator="lessThan">
-      <formula>H24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO26">
+      <formula>H26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO27">
     <cfRule type="cellIs" dxfId="1" priority="755" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="756" operator="lessThan">
-      <formula>H26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO27">
+      <formula>H27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO29">
     <cfRule type="cellIs" dxfId="1" priority="761" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="762" operator="lessThan">
-      <formula>H27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO29">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AO30">
     <cfRule type="cellIs" dxfId="1" priority="767" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="768" operator="lessThan">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AO30">
-    <cfRule type="cellIs" dxfId="1" priority="773" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="774" operator="lessThan">
       <formula>H30</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11760,43 +11696,35 @@
       <formula>AO23</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AP24">
+  <conditionalFormatting sqref="AP26">
     <cfRule type="expression" dxfId="3" priority="751">
-      <formula>AND(AP24&gt;0,AP24&lt;15000)</formula>
+      <formula>AND(AP26&gt;0,AP26&lt;15000)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="752" operator="greaterThan">
-      <formula>AO24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP26">
+      <formula>AO26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP27">
     <cfRule type="expression" dxfId="3" priority="757">
-      <formula>AND(AP26&gt;0,AP26&lt;15000)</formula>
+      <formula>AND(AP27&gt;0,AP27&lt;3000)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="758" operator="greaterThan">
-      <formula>AO26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP27">
+      <formula>AO27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP29">
     <cfRule type="expression" dxfId="3" priority="763">
-      <formula>AND(AP27&gt;0,AP27&lt;3000)</formula>
+      <formula>AND(AP29&gt;0,AP29&lt;25)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="764" operator="greaterThan">
-      <formula>AO27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP29">
+      <formula>AO29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AP30">
     <cfRule type="expression" dxfId="3" priority="769">
-      <formula>AND(AP29&gt;0,AP29&lt;25)</formula>
+      <formula>AND(AP30&gt;0,AP30&lt;3000)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="770" operator="greaterThan">
-      <formula>AO29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AP30">
-    <cfRule type="expression" dxfId="3" priority="775">
-      <formula>AND(AP30&gt;0,AP30&lt;3000)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="776" operator="greaterThan">
       <formula>AO30</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11830,28 +11758,23 @@
       <formula>I23</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AQ24">
+  <conditionalFormatting sqref="AQ26">
     <cfRule type="cellIs" dxfId="4" priority="754" operator="lessThanOrEqual">
-      <formula>I24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ26">
+      <formula>I26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ27">
     <cfRule type="cellIs" dxfId="4" priority="760" operator="lessThanOrEqual">
-      <formula>I26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ27">
+      <formula>I27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ29">
     <cfRule type="cellIs" dxfId="4" priority="766" operator="lessThanOrEqual">
-      <formula>I27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ29">
+      <formula>I29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AQ30">
     <cfRule type="cellIs" dxfId="4" priority="772" operator="lessThanOrEqual">
-      <formula>I29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AQ30">
-    <cfRule type="cellIs" dxfId="4" priority="778" operator="lessThanOrEqual">
       <formula>I30</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11885,28 +11808,23 @@
       <formula>J23</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AR24">
+  <conditionalFormatting sqref="AR26">
     <cfRule type="cellIs" dxfId="4" priority="753" operator="lessThanOrEqual">
-      <formula>J24</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR26">
+      <formula>J26</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR27">
     <cfRule type="cellIs" dxfId="4" priority="759" operator="lessThanOrEqual">
-      <formula>J26</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR27">
+      <formula>J27</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR29">
     <cfRule type="cellIs" dxfId="4" priority="765" operator="lessThanOrEqual">
-      <formula>J27</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR29">
+      <formula>J29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AR30">
     <cfRule type="cellIs" dxfId="4" priority="771" operator="lessThanOrEqual">
-      <formula>J29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AR30">
-    <cfRule type="cellIs" dxfId="4" priority="777" operator="lessThanOrEqual">
       <formula>J30</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11916,126 +11834,126 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT15">
-    <cfRule type="cellIs" dxfId="1" priority="785" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="779" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="786" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="780" operator="lessThan">
       <formula>H15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AT19">
+    <cfRule type="cellIs" dxfId="1" priority="784" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="785" operator="lessThan">
+      <formula>H19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT29">
     <cfRule type="cellIs" dxfId="1" priority="790" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="791" operator="lessThan">
-      <formula>H19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT29">
+      <formula>H29</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT33">
     <cfRule type="cellIs" dxfId="1" priority="796" operator="equal">
       <formula>0</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="797" operator="lessThan">
-      <formula>H29</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT33">
-    <cfRule type="cellIs" dxfId="1" priority="802" operator="equal">
+      <formula>H33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT7">
+    <cfRule type="cellIs" dxfId="1" priority="773" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="803" operator="lessThan">
-      <formula>H33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AT7">
-    <cfRule type="cellIs" dxfId="1" priority="779" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="780" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="774" operator="lessThan">
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU15">
+    <cfRule type="cellIs" dxfId="1" priority="781" operator="greaterThan">
+      <formula>AT15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU19">
+    <cfRule type="expression" dxfId="3" priority="786">
+      <formula>AND(AU19&gt;0,AU19&lt;10)</formula>
+    </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="787" operator="greaterThan">
-      <formula>AT15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU19">
+      <formula>AT19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU29">
     <cfRule type="expression" dxfId="3" priority="792">
-      <formula>AND(AU19&gt;0,AU19&lt;10)</formula>
+      <formula>AND(AU29&gt;0,AU29&lt;3)</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="793" operator="greaterThan">
-      <formula>AT19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AU29">
-    <cfRule type="expression" dxfId="3" priority="798">
-      <formula>AND(AU29&gt;0,AU29&lt;3)</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="799" operator="greaterThan">
       <formula>AT29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU33">
-    <cfRule type="cellIs" dxfId="1" priority="804" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="798" operator="greaterThan">
       <formula>AT33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU7">
-    <cfRule type="expression" dxfId="3" priority="781">
+    <cfRule type="expression" dxfId="3" priority="775">
       <formula>AND(AU7&gt;0,AU7&lt;1800)</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="782" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="776" operator="greaterThan">
       <formula>AT7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV15">
+    <cfRule type="cellIs" dxfId="4" priority="783" operator="lessThanOrEqual">
+      <formula>I15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV19">
     <cfRule type="cellIs" dxfId="4" priority="789" operator="lessThanOrEqual">
-      <formula>I15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV19">
+      <formula>I19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AV29">
     <cfRule type="cellIs" dxfId="4" priority="795" operator="lessThanOrEqual">
-      <formula>I19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AV29">
-    <cfRule type="cellIs" dxfId="4" priority="801" operator="lessThanOrEqual">
       <formula>I29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV33">
-    <cfRule type="cellIs" dxfId="4" priority="806" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="800" operator="lessThanOrEqual">
       <formula>I33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AV7">
-    <cfRule type="cellIs" dxfId="4" priority="784" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="778" operator="lessThanOrEqual">
       <formula>I7</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW15">
+    <cfRule type="cellIs" dxfId="4" priority="782" operator="lessThanOrEqual">
+      <formula>J15</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW19">
     <cfRule type="cellIs" dxfId="4" priority="788" operator="lessThanOrEqual">
-      <formula>J15</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW19">
+      <formula>J19</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AW29">
     <cfRule type="cellIs" dxfId="4" priority="794" operator="lessThanOrEqual">
-      <formula>J19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AW29">
-    <cfRule type="cellIs" dxfId="4" priority="800" operator="lessThanOrEqual">
       <formula>J29</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW33">
-    <cfRule type="cellIs" dxfId="4" priority="805" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="799" operator="lessThanOrEqual">
       <formula>J33</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AW7">
-    <cfRule type="cellIs" dxfId="4" priority="783" operator="lessThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="777" operator="lessThanOrEqual">
       <formula>J7</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13911,80 +13829,79 @@
     <hyperlink ref="AD24" r:id="rId93"/>
     <hyperlink ref="AI24" r:id="rId94"/>
     <hyperlink ref="AN24" r:id="rId95"/>
-    <hyperlink ref="AS24" r:id="rId96"/>
-    <hyperlink ref="G25" r:id="rId97"/>
-    <hyperlink ref="T25" r:id="rId98"/>
-    <hyperlink ref="Y25" r:id="rId99"/>
-    <hyperlink ref="AI25" r:id="rId100"/>
-    <hyperlink ref="AN25" r:id="rId101"/>
-    <hyperlink ref="G26" r:id="rId102"/>
-    <hyperlink ref="T26" r:id="rId103"/>
-    <hyperlink ref="Y26" r:id="rId104"/>
-    <hyperlink ref="AD26" r:id="rId105"/>
-    <hyperlink ref="AI26" r:id="rId106"/>
-    <hyperlink ref="AN26" r:id="rId107"/>
-    <hyperlink ref="AS26" r:id="rId108"/>
-    <hyperlink ref="G27" r:id="rId109"/>
-    <hyperlink ref="T27" r:id="rId110"/>
-    <hyperlink ref="Y27" r:id="rId111"/>
-    <hyperlink ref="AI27" r:id="rId112"/>
-    <hyperlink ref="AN27" r:id="rId113"/>
-    <hyperlink ref="AS27" r:id="rId114"/>
-    <hyperlink ref="G28" r:id="rId115"/>
-    <hyperlink ref="T28" r:id="rId116"/>
-    <hyperlink ref="AD28" r:id="rId117"/>
-    <hyperlink ref="AI28" r:id="rId118"/>
-    <hyperlink ref="G29" r:id="rId119"/>
-    <hyperlink ref="T29" r:id="rId120"/>
-    <hyperlink ref="Y29" r:id="rId121"/>
-    <hyperlink ref="AI29" r:id="rId122"/>
-    <hyperlink ref="AN29" r:id="rId123"/>
-    <hyperlink ref="AS29" r:id="rId124"/>
-    <hyperlink ref="AX29" r:id="rId125"/>
-    <hyperlink ref="G30" r:id="rId126"/>
-    <hyperlink ref="T30" r:id="rId127"/>
-    <hyperlink ref="Y30" r:id="rId128"/>
-    <hyperlink ref="AI30" r:id="rId129"/>
-    <hyperlink ref="AN30" r:id="rId130"/>
-    <hyperlink ref="AS30" r:id="rId131"/>
-    <hyperlink ref="G31" r:id="rId132"/>
-    <hyperlink ref="T31" r:id="rId133"/>
-    <hyperlink ref="Y31" r:id="rId134"/>
-    <hyperlink ref="AI31" r:id="rId135"/>
-    <hyperlink ref="G32" r:id="rId136"/>
-    <hyperlink ref="T32" r:id="rId137"/>
-    <hyperlink ref="Y32" r:id="rId138"/>
-    <hyperlink ref="AI32" r:id="rId139"/>
-    <hyperlink ref="AN32" r:id="rId140"/>
-    <hyperlink ref="G33" r:id="rId141"/>
-    <hyperlink ref="T33" r:id="rId142"/>
-    <hyperlink ref="AI33" r:id="rId143"/>
-    <hyperlink ref="AX33" r:id="rId144"/>
-    <hyperlink ref="G34" r:id="rId145"/>
-    <hyperlink ref="T34" r:id="rId146"/>
-    <hyperlink ref="Y34" r:id="rId147"/>
-    <hyperlink ref="AI34" r:id="rId148"/>
-    <hyperlink ref="AN34" r:id="rId149"/>
-    <hyperlink ref="G35" r:id="rId150"/>
-    <hyperlink ref="T35" r:id="rId151"/>
-    <hyperlink ref="Y35" r:id="rId152"/>
-    <hyperlink ref="AD35" r:id="rId153"/>
-    <hyperlink ref="AI35" r:id="rId154"/>
-    <hyperlink ref="AN35" r:id="rId155"/>
-    <hyperlink ref="G36" r:id="rId156"/>
-    <hyperlink ref="T36" r:id="rId157"/>
-    <hyperlink ref="AI36" r:id="rId158"/>
-    <hyperlink ref="G37" r:id="rId159"/>
-    <hyperlink ref="K39" r:id="rId160"/>
-    <hyperlink ref="P39" r:id="rId161"/>
-    <hyperlink ref="U39" r:id="rId162"/>
-    <hyperlink ref="Z39" r:id="rId163"/>
-    <hyperlink ref="AE39" r:id="rId164"/>
-    <hyperlink ref="AJ39" r:id="rId165"/>
-    <hyperlink ref="AO39" r:id="rId166"/>
-    <hyperlink ref="AT39" r:id="rId167"/>
+    <hyperlink ref="G25" r:id="rId96"/>
+    <hyperlink ref="T25" r:id="rId97"/>
+    <hyperlink ref="Y25" r:id="rId98"/>
+    <hyperlink ref="AI25" r:id="rId99"/>
+    <hyperlink ref="AN25" r:id="rId100"/>
+    <hyperlink ref="G26" r:id="rId101"/>
+    <hyperlink ref="T26" r:id="rId102"/>
+    <hyperlink ref="Y26" r:id="rId103"/>
+    <hyperlink ref="AD26" r:id="rId104"/>
+    <hyperlink ref="AI26" r:id="rId105"/>
+    <hyperlink ref="AN26" r:id="rId106"/>
+    <hyperlink ref="AS26" r:id="rId107"/>
+    <hyperlink ref="G27" r:id="rId108"/>
+    <hyperlink ref="T27" r:id="rId109"/>
+    <hyperlink ref="Y27" r:id="rId110"/>
+    <hyperlink ref="AI27" r:id="rId111"/>
+    <hyperlink ref="AN27" r:id="rId112"/>
+    <hyperlink ref="AS27" r:id="rId113"/>
+    <hyperlink ref="G28" r:id="rId114"/>
+    <hyperlink ref="T28" r:id="rId115"/>
+    <hyperlink ref="AD28" r:id="rId116"/>
+    <hyperlink ref="AI28" r:id="rId117"/>
+    <hyperlink ref="G29" r:id="rId118"/>
+    <hyperlink ref="T29" r:id="rId119"/>
+    <hyperlink ref="Y29" r:id="rId120"/>
+    <hyperlink ref="AI29" r:id="rId121"/>
+    <hyperlink ref="AN29" r:id="rId122"/>
+    <hyperlink ref="AS29" r:id="rId123"/>
+    <hyperlink ref="AX29" r:id="rId124"/>
+    <hyperlink ref="G30" r:id="rId125"/>
+    <hyperlink ref="T30" r:id="rId126"/>
+    <hyperlink ref="Y30" r:id="rId127"/>
+    <hyperlink ref="AI30" r:id="rId128"/>
+    <hyperlink ref="AN30" r:id="rId129"/>
+    <hyperlink ref="AS30" r:id="rId130"/>
+    <hyperlink ref="G31" r:id="rId131"/>
+    <hyperlink ref="T31" r:id="rId132"/>
+    <hyperlink ref="Y31" r:id="rId133"/>
+    <hyperlink ref="AI31" r:id="rId134"/>
+    <hyperlink ref="G32" r:id="rId135"/>
+    <hyperlink ref="T32" r:id="rId136"/>
+    <hyperlink ref="Y32" r:id="rId137"/>
+    <hyperlink ref="AI32" r:id="rId138"/>
+    <hyperlink ref="AN32" r:id="rId139"/>
+    <hyperlink ref="G33" r:id="rId140"/>
+    <hyperlink ref="T33" r:id="rId141"/>
+    <hyperlink ref="AI33" r:id="rId142"/>
+    <hyperlink ref="AX33" r:id="rId143"/>
+    <hyperlink ref="G34" r:id="rId144"/>
+    <hyperlink ref="T34" r:id="rId145"/>
+    <hyperlink ref="Y34" r:id="rId146"/>
+    <hyperlink ref="AI34" r:id="rId147"/>
+    <hyperlink ref="AN34" r:id="rId148"/>
+    <hyperlink ref="G35" r:id="rId149"/>
+    <hyperlink ref="T35" r:id="rId150"/>
+    <hyperlink ref="Y35" r:id="rId151"/>
+    <hyperlink ref="AD35" r:id="rId152"/>
+    <hyperlink ref="AI35" r:id="rId153"/>
+    <hyperlink ref="AN35" r:id="rId154"/>
+    <hyperlink ref="G36" r:id="rId155"/>
+    <hyperlink ref="T36" r:id="rId156"/>
+    <hyperlink ref="AI36" r:id="rId157"/>
+    <hyperlink ref="G37" r:id="rId158"/>
+    <hyperlink ref="K39" r:id="rId159"/>
+    <hyperlink ref="P39" r:id="rId160"/>
+    <hyperlink ref="U39" r:id="rId161"/>
+    <hyperlink ref="Z39" r:id="rId162"/>
+    <hyperlink ref="AE39" r:id="rId163"/>
+    <hyperlink ref="AJ39" r:id="rId164"/>
+    <hyperlink ref="AO39" r:id="rId165"/>
+    <hyperlink ref="AT39" r:id="rId166"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId168"/>
+  <legacyDrawing r:id="rId167"/>
 </worksheet>
 </file>
</xml_diff>